<commit_message>
normalize operational data with linear interpolation
</commit_message>
<xml_diff>
--- a/org.xtext.example.Adeptness/resources/TrainingData_MiercolesSur_trainingdata1.xlsx
+++ b/org.xtext.example.Adeptness/resources/TrainingData_MiercolesSur_trainingdata1.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox (MGEP)\ADEPTNESS_Aitor\OraculosIA\instalaciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\AdeptnessDSL\org.xtext.example.Adeptness\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04302B24-194F-4E50-8B69-9938B880660D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>UP</t>
   </si>
@@ -43,11 +53,14 @@
   <si>
     <t>ATTD</t>
   </si>
+  <si>
+    <t>timestamp</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,2220 +372,2539 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F105"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F105"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
       <c r="C2">
-        <f>SUM(A2:B2)</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>SUM(A2:C2)</f>
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>3.3333333329999999E-2</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>57.45</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>57.483333330000001</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C66" si="0">SUM(A3:B3)</f>
-        <v>6</v>
-      </c>
       <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">SUM(A3:C3)</f>
+        <v>7</v>
+      </c>
+      <c r="E3">
         <v>3.1</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>40.383333329999999</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>43.483333330000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
       <c r="D4">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+      <c r="E4">
         <v>5.4</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>40.644444440000001</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>46.044444439999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
       <c r="D5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E5">
         <v>10.84285714</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>59.728571430000002</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>70.571428569999995</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
       <c r="D6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E6">
         <v>15.025</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>52.625</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>67.650000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7">
         <v>0</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
       <c r="D7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E7">
         <v>10.9</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>63.3</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>74.2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
       <c r="D8">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+      <c r="E8">
         <v>17.43333333</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>44.116666670000001</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>61.55</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="C9">
         <v>1</v>
       </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
       <c r="D9">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="E9">
         <v>11.46</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>49.72</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>61.18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10">
         <v>1</v>
       </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
       <c r="D10">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E10">
         <v>13.3</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>53.64</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>66.94</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>14</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
+        <v>8.99</v>
+      </c>
+      <c r="C11">
         <v>0</v>
       </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
       <c r="D11">
+        <f t="shared" si="0"/>
+        <v>22.990000000000002</v>
+      </c>
+      <c r="E11">
         <v>9.9285714289999998</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>61.214285709999999</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>71.142857140000004</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>13</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="C12">
         <v>4</v>
       </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
       <c r="D12">
+        <f t="shared" si="0"/>
+        <v>26.5</v>
+      </c>
+      <c r="E12">
         <v>9.1705882350000003</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>68.752941179999993</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>77.92352941</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>18</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
+        <v>10.89</v>
+      </c>
+      <c r="C13">
         <v>2</v>
       </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
       <c r="D13">
+        <f t="shared" si="0"/>
+        <v>30.89</v>
+      </c>
+      <c r="E13">
         <v>10.14</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>53.045000000000002</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>63.185000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>18</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
+        <v>12</v>
+      </c>
+      <c r="C14">
         <v>1</v>
       </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
       <c r="D14">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="E14">
         <v>6.268421053</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>90.715789470000004</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>96.984210529999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>23</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
+        <v>13</v>
+      </c>
+      <c r="C15">
         <v>0</v>
       </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
       <c r="D15">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E15">
         <v>8.8913043480000002</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>83.069565220000001</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>91.96086957</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>25</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
+        <v>14</v>
+      </c>
+      <c r="C16">
         <v>5</v>
       </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
       <c r="D16">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E16">
         <v>7.4766666669999999</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>67.573333329999997</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>75.05</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>29</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
+        <v>14.8</v>
+      </c>
+      <c r="C17">
         <v>2</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
       <c r="D17">
+        <f t="shared" si="0"/>
+        <v>45.8</v>
+      </c>
+      <c r="E17">
         <v>7.0354838710000003</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>84.096774190000005</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>91.132258059999998</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>26</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
+        <v>15.86</v>
+      </c>
+      <c r="C18">
         <v>4</v>
       </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
       <c r="D18">
+        <f t="shared" si="0"/>
+        <v>45.86</v>
+      </c>
+      <c r="E18">
         <v>10.50666667</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>62.653333330000002</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>73.16</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>25</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
+        <v>17</v>
+      </c>
+      <c r="C19">
         <v>2</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
       <c r="D19">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E19">
         <v>12.996296299999999</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>56.388888889999997</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>69.385185190000001</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>33</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
+        <v>18</v>
+      </c>
+      <c r="C20">
         <v>1</v>
       </c>
-      <c r="C20">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
       <c r="D20">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="E20">
         <v>10.60882353</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>80.964705879999997</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>91.573529410000006</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>38</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="C21">
         <v>3</v>
       </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
       <c r="D21">
+        <f t="shared" si="0"/>
+        <v>59.9</v>
+      </c>
+      <c r="E21">
         <v>3.7439024390000002</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>89.153658539999995</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>92.897560979999994</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>30</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
+        <v>20</v>
+      </c>
+      <c r="C22">
         <v>5</v>
       </c>
-      <c r="C22">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
       <c r="D22">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="E22">
         <v>9.5628571430000004</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>68.017142860000007</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>77.58</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>25</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
+        <v>21</v>
+      </c>
+      <c r="C23">
         <v>4</v>
       </c>
-      <c r="C23">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
       <c r="D23">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E23">
         <v>7.5793103449999997</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>62.413793099999999</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>69.993103450000007</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>38</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
+        <v>22</v>
+      </c>
+      <c r="C24">
         <v>5</v>
       </c>
-      <c r="C24">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
       <c r="D24">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="E24">
         <v>8.0581395350000005</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>84.786046510000006</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>92.844186050000005</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>40</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
+        <v>23</v>
+      </c>
+      <c r="C25">
         <v>4</v>
       </c>
-      <c r="C25">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
       <c r="D25">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="E25">
         <v>6.4295454550000004</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>75.679545450000006</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>82.109090910000006</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>40</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
+        <v>24</v>
+      </c>
+      <c r="C26">
         <v>5</v>
       </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
       <c r="D26">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="E26">
         <v>7.448888889</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>86.208888889999997</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>93.657777780000004</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>59</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
+        <v>25</v>
+      </c>
+      <c r="C27">
         <v>10</v>
       </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
       <c r="D27">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="E27">
         <v>6.7927536230000003</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>107.1188406</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>113.9115942</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>44</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
+        <v>26</v>
+      </c>
+      <c r="C28">
         <v>3</v>
       </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
       <c r="D28">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="E28">
         <v>6.2361702130000003</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>107.2297872</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>113.46595739999999</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>47</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
+        <v>27</v>
+      </c>
+      <c r="C29">
         <v>4</v>
       </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
       <c r="D29">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="E29">
         <v>7.1666666670000003</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>82.460784309999994</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>89.627450980000006</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>44</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
+        <v>28</v>
+      </c>
+      <c r="C30">
         <v>11</v>
       </c>
-      <c r="C30">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
       <c r="D30">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="E30">
         <v>7.1890909089999999</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>81.409090910000003</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>88.598181819999994</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>59</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
+        <v>29</v>
+      </c>
+      <c r="C31">
         <v>10</v>
       </c>
-      <c r="C31">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
       <c r="D31">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="E31">
         <v>7.5333333329999999</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>93.597101449999997</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>101.1304348</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>46</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
+        <v>30</v>
+      </c>
+      <c r="C32">
         <v>11</v>
       </c>
-      <c r="C32">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
       <c r="D32">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="E32">
         <v>9.1859649119999993</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>80.145614039999998</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>89.331578949999994</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>42</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
+        <v>31</v>
+      </c>
+      <c r="C33">
         <v>12</v>
       </c>
-      <c r="C33">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
       <c r="D33">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="E33">
         <v>7.9537037039999996</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>74.962962959999999</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>82.916666669999998</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>56</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
+        <v>32</v>
+      </c>
+      <c r="C34">
         <v>14</v>
       </c>
-      <c r="C34">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
       <c r="D34">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+      <c r="E34">
         <v>7.6385714289999997</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>87.414285710000001</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>95.05285714</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>41</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
+        <v>33</v>
+      </c>
+      <c r="C35">
         <v>11</v>
       </c>
-      <c r="C35">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
       <c r="D35">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="E35">
         <v>7.5461538460000002</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>75.590384619999995</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>83.136538459999997</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>39</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
+        <v>34</v>
+      </c>
+      <c r="C36">
         <v>11</v>
       </c>
-      <c r="C36">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
       <c r="D36">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="E36">
         <v>2.3959999999999999</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>86.882000000000005</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>89.278000000000006</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>53</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
+        <v>35</v>
+      </c>
+      <c r="C37">
         <v>20</v>
       </c>
-      <c r="C37">
-        <f t="shared" si="0"/>
-        <v>73</v>
-      </c>
       <c r="D37">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="E37">
         <v>8.9917808220000008</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>75.015068490000004</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>84.006849320000001</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>39</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
+        <v>36</v>
+      </c>
+      <c r="C38">
         <v>16</v>
       </c>
-      <c r="C38">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
       <c r="D38">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="E38">
         <v>12.06</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>62.370909089999998</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>74.43090909</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
+        <v>37</v>
+      </c>
+      <c r="C39">
         <v>15</v>
       </c>
-      <c r="C39">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
       <c r="D39">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="E39">
         <v>6.5943396229999998</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>59.375471699999999</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>65.969811320000005</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
+        <v>38</v>
+      </c>
+      <c r="C40">
         <v>16</v>
       </c>
-      <c r="C40">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
       <c r="D40">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="E40">
         <v>8.6703703700000005</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>56.951851849999997</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>65.622222219999998</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>21</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
+        <v>39</v>
+      </c>
+      <c r="C41">
         <v>14</v>
       </c>
-      <c r="C41">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
       <c r="D41">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="E41">
         <v>4.1028571429999996</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>62.065714290000003</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>66.16857143</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>24</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
+        <v>40</v>
+      </c>
+      <c r="C42">
         <v>10</v>
       </c>
-      <c r="C42">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
       <c r="D42">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="E42">
         <v>12.08529412</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>53.58235294</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>65.667647059999993</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>32</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
+        <v>41</v>
+      </c>
+      <c r="C43">
         <v>17</v>
       </c>
-      <c r="C43">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
       <c r="D43">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="E43">
         <v>8.1857142859999996</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>47.867346939999997</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>56.053061219999996</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>23</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
+        <v>42</v>
+      </c>
+      <c r="C44">
         <v>13</v>
       </c>
-      <c r="C44">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
       <c r="D44">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="E44">
         <v>10.89722222</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>57.019444440000001</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>67.916666669999998</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>24</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
+        <v>43</v>
+      </c>
+      <c r="C45">
         <v>17</v>
       </c>
-      <c r="C45">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
       <c r="D45">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="E45">
         <v>6.1780487800000001</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>47.921951219999997</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>54.1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>28</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
+        <v>44</v>
+      </c>
+      <c r="C46">
         <v>16</v>
       </c>
-      <c r="C46">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
       <c r="D46">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="E46">
         <v>4.7659090910000002</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>60.197727270000001</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>64.963636359999995</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>10</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
+        <v>45</v>
+      </c>
+      <c r="C47">
         <v>19</v>
       </c>
-      <c r="C47">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
       <c r="D47">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="E47">
         <v>6.6793103450000002</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>39.575862069999999</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>46.25517241</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>27</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
+        <v>46</v>
+      </c>
+      <c r="C48">
         <v>24</v>
       </c>
-      <c r="C48">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
       <c r="D48">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="E48">
         <v>10.50784314</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>44.015686270000003</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>54.523529410000002</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>24</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
+        <v>47</v>
+      </c>
+      <c r="C49">
         <v>36</v>
       </c>
-      <c r="C49">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
       <c r="D49">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+      <c r="E49">
         <v>13.855</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>53.854999999999997</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>67.709999999999994</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>28</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
+        <v>48</v>
+      </c>
+      <c r="C50">
         <v>14</v>
       </c>
-      <c r="C50">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
       <c r="D50">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="E50">
         <v>8.7714285709999995</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>68.438095239999996</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>77.209523809999993</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>27</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
+        <v>49</v>
+      </c>
+      <c r="C51">
         <v>24</v>
       </c>
-      <c r="C51">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
       <c r="D51">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="E51">
         <v>11.176470589999999</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>53.19607843</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>64.372549019999994</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>27</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
+        <v>50</v>
+      </c>
+      <c r="C52">
         <v>28</v>
       </c>
-      <c r="C52">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
       <c r="D52">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="E52">
         <v>15.38545455</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>67.147272729999997</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>82.532727269999995</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>18</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
+        <v>51</v>
+      </c>
+      <c r="C53">
         <v>26</v>
       </c>
-      <c r="C53">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
       <c r="D53">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="E53">
         <v>6.8772727270000003</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>51.588636360000002</v>
       </c>
-      <c r="F53">
+      <c r="G53">
         <v>58.465909089999997</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>14</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
+        <v>52</v>
+      </c>
+      <c r="C54">
         <v>13</v>
       </c>
-      <c r="C54">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
       <c r="D54">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="E54">
         <v>6.5037037040000003</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>49.10740741</v>
       </c>
-      <c r="F54">
+      <c r="G54">
         <v>55.611111110000003</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>23</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1">
+        <v>53</v>
+      </c>
+      <c r="C55">
         <v>18</v>
       </c>
-      <c r="C55">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
       <c r="D55">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="E55">
         <v>6.456097561</v>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>58.585365850000002</v>
       </c>
-      <c r="F55">
+      <c r="G55">
         <v>65.041463410000006</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>25</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1">
+        <v>54</v>
+      </c>
+      <c r="C56">
         <v>17</v>
       </c>
-      <c r="C56">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
       <c r="D56">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="E56">
         <v>5.845238095</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>50.735714289999997</v>
       </c>
-      <c r="F56">
+      <c r="G56">
         <v>56.580952379999999</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>21</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1">
+        <v>55</v>
+      </c>
+      <c r="C57">
         <v>17</v>
       </c>
-      <c r="C57">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
       <c r="D57">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="E57">
         <v>7.3421052629999997</v>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>44.70789474</v>
       </c>
-      <c r="F57">
+      <c r="G57">
         <v>52.05</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>31</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1">
+        <v>56</v>
+      </c>
+      <c r="C58">
         <v>12</v>
       </c>
-      <c r="C58">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
       <c r="D58">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="E58">
         <v>5.0418604650000001</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>55.469767439999998</v>
       </c>
-      <c r="F58">
+      <c r="G58">
         <v>60.511627910000001</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>11</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="1">
+        <v>57</v>
+      </c>
+      <c r="C59">
         <v>9</v>
       </c>
-      <c r="C59">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
       <c r="D59">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="E59">
         <v>6.2949999999999999</v>
       </c>
-      <c r="E59">
+      <c r="F59">
         <v>44.405000000000001</v>
       </c>
-      <c r="F59">
+      <c r="G59">
         <v>50.7</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>23</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1">
+        <v>58</v>
+      </c>
+      <c r="C60">
         <v>20</v>
       </c>
-      <c r="C60">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
       <c r="D60">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+      <c r="E60">
         <v>7.3930232560000002</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>48.29069767</v>
       </c>
-      <c r="F60">
+      <c r="G60">
         <v>55.68372093</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>26</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="1">
+        <v>59</v>
+      </c>
+      <c r="C61">
         <v>20</v>
       </c>
-      <c r="C61">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
       <c r="D61">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="E61">
         <v>12.72173913</v>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>49.145652169999998</v>
       </c>
-      <c r="F61">
+      <c r="G61">
         <v>61.867391300000001</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>30</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="1">
+        <v>60</v>
+      </c>
+      <c r="C62">
         <v>35</v>
       </c>
-      <c r="C62">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
       <c r="D62">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="E62">
         <v>15.74</v>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>51.326153849999997</v>
       </c>
-      <c r="F62">
+      <c r="G62">
         <v>67.066153850000006</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>32</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="1">
+        <v>61</v>
+      </c>
+      <c r="C63">
         <v>20</v>
       </c>
-      <c r="C63">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
       <c r="D63">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="E63">
         <v>16.265384619999999</v>
       </c>
-      <c r="E63">
+      <c r="F63">
         <v>53.840384620000002</v>
       </c>
-      <c r="F63">
+      <c r="G63">
         <v>70.105769230000007</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>28</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="1">
+        <v>62</v>
+      </c>
+      <c r="C64">
         <v>7</v>
       </c>
-      <c r="C64">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
       <c r="D64">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="E64">
         <v>5.9942857140000001</v>
       </c>
-      <c r="E64">
+      <c r="F64">
         <v>45.742857139999998</v>
       </c>
-      <c r="F64">
+      <c r="G64">
         <v>51.737142859999999</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>26</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="1">
+        <v>63</v>
+      </c>
+      <c r="C65">
         <v>19</v>
       </c>
-      <c r="C65">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
       <c r="D65">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="E65">
         <v>7.6111111109999996</v>
       </c>
-      <c r="E65">
+      <c r="F65">
         <v>44.211111109999997</v>
       </c>
-      <c r="F65">
+      <c r="G65">
         <v>51.82222222</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>22</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="1">
+        <v>64</v>
+      </c>
+      <c r="C66">
         <v>23</v>
       </c>
-      <c r="C66">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
       <c r="D66">
+        <f t="shared" si="0"/>
+        <v>109</v>
+      </c>
+      <c r="E66">
         <v>7.7777777779999999</v>
       </c>
-      <c r="E66">
+      <c r="F66">
         <v>50.67777778</v>
       </c>
-      <c r="F66">
+      <c r="G66">
         <v>58.455555560000001</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>8</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="1">
+        <v>65</v>
+      </c>
+      <c r="C67">
         <v>13</v>
       </c>
-      <c r="C67">
-        <f t="shared" ref="C67:C105" si="1">SUM(A67:B67)</f>
-        <v>21</v>
-      </c>
       <c r="D67">
+        <f t="shared" ref="D67:D105" si="1">SUM(A67:C67)</f>
+        <v>86</v>
+      </c>
+      <c r="E67">
         <v>7.9857142860000003</v>
       </c>
-      <c r="E67">
+      <c r="F67">
         <v>41</v>
       </c>
-      <c r="F67">
+      <c r="G67">
         <v>48.985714289999997</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>13</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="1">
+        <v>66</v>
+      </c>
+      <c r="C68">
         <v>13</v>
       </c>
-      <c r="C68">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
       <c r="D68">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="E68">
         <v>9.3730769229999993</v>
       </c>
-      <c r="E68">
+      <c r="F68">
         <v>42.784615379999998</v>
       </c>
-      <c r="F68">
+      <c r="G68">
         <v>52.157692310000002</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>23</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="1">
+        <v>67</v>
+      </c>
+      <c r="C69">
         <v>8</v>
       </c>
-      <c r="C69">
-        <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
       <c r="D69">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="E69">
         <v>8.3677419349999997</v>
       </c>
-      <c r="E69">
+      <c r="F69">
         <v>47.235483870000003</v>
       </c>
-      <c r="F69">
+      <c r="G69">
         <v>55.603225809999998</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>14</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="1">
+        <v>68</v>
+      </c>
+      <c r="C70">
         <v>25</v>
       </c>
-      <c r="C70">
-        <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
       <c r="D70">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="E70">
         <v>8.4128205129999998</v>
       </c>
-      <c r="E70">
+      <c r="F70">
         <v>56.438461539999999</v>
       </c>
-      <c r="F70">
+      <c r="G70">
         <v>64.851282049999995</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>8</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="1">
+        <v>69</v>
+      </c>
+      <c r="C71">
         <v>14</v>
       </c>
-      <c r="C71">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
       <c r="D71">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="E71">
         <v>8.5545454549999995</v>
       </c>
-      <c r="E71">
+      <c r="F71">
         <v>55.809090910000002</v>
       </c>
-      <c r="F71">
+      <c r="G71">
         <v>64.363636360000001</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>12</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="1">
+        <v>70</v>
+      </c>
+      <c r="C72">
         <v>6</v>
       </c>
-      <c r="C72">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
       <c r="D72">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="E72">
         <v>4.7777777779999999</v>
       </c>
-      <c r="E72">
+      <c r="F72">
         <v>41.244444440000002</v>
       </c>
-      <c r="F72">
+      <c r="G72">
         <v>46.022222220000003</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>14</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="1">
+        <v>71</v>
+      </c>
+      <c r="C73">
         <v>20</v>
       </c>
-      <c r="C73">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
       <c r="D73">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="E73">
         <v>8.3705882349999996</v>
       </c>
-      <c r="E73">
+      <c r="F73">
         <v>50.861764710000003</v>
       </c>
-      <c r="F73">
+      <c r="G73">
         <v>59.232352939999998</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>20</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="1">
+        <v>72</v>
+      </c>
+      <c r="C74">
         <v>37</v>
       </c>
-      <c r="C74">
-        <f t="shared" si="1"/>
-        <v>57</v>
-      </c>
       <c r="D74">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="E74">
         <v>9.5964912279999997</v>
       </c>
-      <c r="E74">
+      <c r="F74">
         <v>58.468421050000003</v>
       </c>
-      <c r="F74">
+      <c r="G74">
         <v>68.064912280000001</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>16</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="1">
+        <v>73</v>
+      </c>
+      <c r="C75">
         <v>45</v>
       </c>
-      <c r="C75">
-        <f t="shared" si="1"/>
-        <v>61</v>
-      </c>
       <c r="D75">
+        <f t="shared" si="1"/>
+        <v>134</v>
+      </c>
+      <c r="E75">
         <v>11.244262300000001</v>
       </c>
-      <c r="E75">
+      <c r="F75">
         <v>63.327868850000002</v>
       </c>
-      <c r="F75">
+      <c r="G75">
         <v>74.572131150000004</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>15</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="1">
+        <v>74</v>
+      </c>
+      <c r="C76">
         <v>30</v>
       </c>
-      <c r="C76">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
       <c r="D76">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="E76">
         <v>7.6466666669999999</v>
       </c>
-      <c r="E76">
+      <c r="F76">
         <v>52.853333329999998</v>
       </c>
-      <c r="F76">
+      <c r="G76">
         <v>60.5</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>21</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="1">
+        <v>75</v>
+      </c>
+      <c r="C77">
         <v>41</v>
       </c>
-      <c r="C77">
-        <f t="shared" si="1"/>
-        <v>62</v>
-      </c>
       <c r="D77">
+        <f t="shared" si="1"/>
+        <v>137</v>
+      </c>
+      <c r="E77">
         <v>8.2225806450000007</v>
       </c>
-      <c r="E77">
+      <c r="F77">
         <v>59.079032259999998</v>
       </c>
-      <c r="F77">
+      <c r="G77">
         <v>67.301612899999995</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>8</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="1">
+        <v>76</v>
+      </c>
+      <c r="C78">
         <v>33</v>
       </c>
-      <c r="C78">
-        <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
       <c r="D78">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="E78">
         <v>12.70731707</v>
       </c>
-      <c r="E78">
+      <c r="F78">
         <v>51.190243899999999</v>
       </c>
-      <c r="F78">
+      <c r="G78">
         <v>63.897560980000002</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>10</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="1">
+        <v>77</v>
+      </c>
+      <c r="C79">
         <v>43</v>
       </c>
-      <c r="C79">
-        <f t="shared" si="1"/>
-        <v>53</v>
-      </c>
       <c r="D79">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="E79">
         <v>13.50754717</v>
       </c>
-      <c r="E79">
+      <c r="F79">
         <v>46.847169809999997</v>
       </c>
-      <c r="F79">
+      <c r="G79">
         <v>60.354716979999999</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>16</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="1">
+        <v>78</v>
+      </c>
+      <c r="C80">
         <v>35</v>
       </c>
-      <c r="C80">
-        <f t="shared" si="1"/>
-        <v>51</v>
-      </c>
       <c r="D80">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="E80">
         <v>7.2764705879999996</v>
       </c>
-      <c r="E80">
+      <c r="F80">
         <v>48.637254900000002</v>
       </c>
-      <c r="F80">
+      <c r="G80">
         <v>55.913725489999997</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>19</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="1">
+        <v>79</v>
+      </c>
+      <c r="C81">
         <v>28</v>
       </c>
-      <c r="C81">
-        <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
       <c r="D81">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="E81">
         <v>8.9723404260000006</v>
       </c>
-      <c r="E81">
+      <c r="F81">
         <v>49.889361700000002</v>
       </c>
-      <c r="F81">
+      <c r="G81">
         <v>58.861702129999998</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>19</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="1">
+        <v>80</v>
+      </c>
+      <c r="C82">
         <v>33</v>
       </c>
-      <c r="C82">
-        <f t="shared" si="1"/>
-        <v>52</v>
-      </c>
       <c r="D82">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+      <c r="E82">
         <v>11.16923077</v>
       </c>
-      <c r="E82">
+      <c r="F82">
         <v>49.976923079999999</v>
       </c>
-      <c r="F82">
+      <c r="G82">
         <v>61.146153849999997</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>12</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="1">
+        <v>81</v>
+      </c>
+      <c r="C83">
         <v>51</v>
       </c>
-      <c r="C83">
-        <f t="shared" si="1"/>
-        <v>63</v>
-      </c>
       <c r="D83">
+        <f t="shared" si="1"/>
+        <v>144</v>
+      </c>
+      <c r="E83">
         <v>14.21587302</v>
       </c>
-      <c r="E83">
+      <c r="F83">
         <v>46.666666669999998</v>
       </c>
-      <c r="F83">
+      <c r="G83">
         <v>60.882539680000001</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>18</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="1">
+        <v>82</v>
+      </c>
+      <c r="C84">
         <v>18</v>
       </c>
-      <c r="C84">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
       <c r="D84">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="E84">
         <v>9.5749999999999993</v>
       </c>
-      <c r="E84">
+      <c r="F84">
         <v>45.438888890000001</v>
       </c>
-      <c r="F84">
+      <c r="G84">
         <v>55.013888889999997</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>19</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="1">
+        <v>83</v>
+      </c>
+      <c r="C85">
         <v>26</v>
       </c>
-      <c r="C85">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
       <c r="D85">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="E85">
         <v>10.50222222</v>
       </c>
-      <c r="E85">
+      <c r="F85">
         <v>50.27111111</v>
       </c>
-      <c r="F85">
+      <c r="G85">
         <v>60.77333333</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>35</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="1">
+        <v>84</v>
+      </c>
+      <c r="C86">
         <v>58</v>
       </c>
-      <c r="C86">
-        <f t="shared" si="1"/>
-        <v>93</v>
-      </c>
       <c r="D86">
+        <f t="shared" si="1"/>
+        <v>177</v>
+      </c>
+      <c r="E86">
         <v>9.2440860219999994</v>
       </c>
-      <c r="E86">
+      <c r="F86">
         <v>55.113978490000001</v>
       </c>
-      <c r="F86">
+      <c r="G86">
         <v>64.358064519999999</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>32</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="1">
+        <v>85</v>
+      </c>
+      <c r="C87">
         <v>49</v>
       </c>
-      <c r="C87">
-        <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
       <c r="D87">
+        <f t="shared" si="1"/>
+        <v>166</v>
+      </c>
+      <c r="E87">
         <v>10.08024691</v>
       </c>
-      <c r="E87">
+      <c r="F87">
         <v>57.67777778</v>
       </c>
-      <c r="F87">
+      <c r="G87">
         <v>67.758024689999999</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>31</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="1">
+        <v>86</v>
+      </c>
+      <c r="C88">
         <v>43</v>
       </c>
-      <c r="C88">
-        <f t="shared" si="1"/>
-        <v>74</v>
-      </c>
       <c r="D88">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="E88">
         <v>13.917567569999999</v>
       </c>
-      <c r="E88">
+      <c r="F88">
         <v>72.606756759999996</v>
       </c>
-      <c r="F88">
+      <c r="G88">
         <v>86.524324320000005</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>60</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="1">
+        <v>87</v>
+      </c>
+      <c r="C89">
         <v>44</v>
       </c>
-      <c r="C89">
-        <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
       <c r="D89">
+        <f t="shared" si="1"/>
+        <v>191</v>
+      </c>
+      <c r="E89">
         <v>20.94038462</v>
       </c>
-      <c r="E89">
+      <c r="F89">
         <v>73.533653849999993</v>
       </c>
-      <c r="F89">
+      <c r="G89">
         <v>94.474038460000003</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>37</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="1">
+        <v>88</v>
+      </c>
+      <c r="C90">
         <v>23</v>
       </c>
-      <c r="C90">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
       <c r="D90">
+        <f t="shared" si="1"/>
+        <v>148</v>
+      </c>
+      <c r="E90">
         <v>7.1566666669999996</v>
       </c>
-      <c r="E90">
+      <c r="F90">
         <v>55.65</v>
       </c>
-      <c r="F90">
+      <c r="G90">
         <v>62.806666669999998</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>42</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="1">
+        <v>89</v>
+      </c>
+      <c r="C91">
         <v>21</v>
       </c>
-      <c r="C91">
-        <f t="shared" si="1"/>
-        <v>63</v>
-      </c>
       <c r="D91">
+        <f t="shared" si="1"/>
+        <v>152</v>
+      </c>
+      <c r="E91">
         <v>8.7523809519999993</v>
       </c>
-      <c r="E91">
+      <c r="F91">
         <v>61.485714289999997</v>
       </c>
-      <c r="F91">
+      <c r="G91">
         <v>70.238095240000007</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>18</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="1">
+        <v>90</v>
+      </c>
+      <c r="C92">
         <v>24</v>
       </c>
-      <c r="C92">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
       <c r="D92">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+      <c r="E92">
         <v>7.7285714289999996</v>
       </c>
-      <c r="E92">
+      <c r="F92">
         <v>53.4</v>
       </c>
-      <c r="F92">
+      <c r="G92">
         <v>61.128571430000001</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>15</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="1">
+        <v>91</v>
+      </c>
+      <c r="C93">
         <v>20</v>
       </c>
-      <c r="C93">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
       <c r="D93">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="E93">
         <v>6.6371428569999997</v>
       </c>
-      <c r="E93">
+      <c r="F93">
         <v>44.38</v>
       </c>
-      <c r="F93">
+      <c r="G93">
         <v>51.01714286</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>21</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="1">
+        <v>92</v>
+      </c>
+      <c r="C94">
         <v>11</v>
       </c>
-      <c r="C94">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
       <c r="D94">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="E94">
         <v>4.859375</v>
       </c>
-      <c r="E94">
+      <c r="F94">
         <v>53.315624999999997</v>
       </c>
-      <c r="F94">
+      <c r="G94">
         <v>58.174999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>23</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="1">
+        <v>93</v>
+      </c>
+      <c r="C95">
         <v>15</v>
       </c>
-      <c r="C95">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
       <c r="D95">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="E95">
         <v>8.0657894740000007</v>
       </c>
-      <c r="E95">
+      <c r="F95">
         <v>63.215789469999997</v>
       </c>
-      <c r="F95">
+      <c r="G95">
         <v>71.281578949999997</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>21</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="1">
+        <v>94</v>
+      </c>
+      <c r="C96">
         <v>7</v>
       </c>
-      <c r="C96">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
       <c r="D96">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="E96">
         <v>3.5714285710000002</v>
       </c>
-      <c r="E96">
+      <c r="F96">
         <v>57.982142860000003</v>
       </c>
-      <c r="F96">
+      <c r="G96">
         <v>61.553571429999998</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>32</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="1">
+        <v>95</v>
+      </c>
+      <c r="C97">
         <v>19</v>
       </c>
-      <c r="C97">
-        <f t="shared" si="1"/>
-        <v>51</v>
-      </c>
       <c r="D97">
+        <f t="shared" si="1"/>
+        <v>146</v>
+      </c>
+      <c r="E97">
         <v>8.1431372549999992</v>
       </c>
-      <c r="E97">
+      <c r="F97">
         <v>63.950980389999998</v>
       </c>
-      <c r="F97">
+      <c r="G97">
         <v>72.094117650000001</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>74</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="1">
+        <v>96</v>
+      </c>
+      <c r="C98">
         <v>39</v>
       </c>
-      <c r="C98">
-        <f t="shared" si="1"/>
-        <v>113</v>
-      </c>
       <c r="D98">
+        <f t="shared" si="1"/>
+        <v>209</v>
+      </c>
+      <c r="E98">
         <v>18.784070799999999</v>
       </c>
-      <c r="E98">
+      <c r="F98">
         <v>72.691150440000001</v>
       </c>
-      <c r="F98">
+      <c r="G98">
         <v>91.475221239999996</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>47</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="1">
+        <v>97</v>
+      </c>
+      <c r="C99">
         <v>41</v>
       </c>
-      <c r="C99">
-        <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
       <c r="D99">
+        <f t="shared" si="1"/>
+        <v>185</v>
+      </c>
+      <c r="E99">
         <v>21.10454545</v>
       </c>
-      <c r="E99">
+      <c r="F99">
         <v>64.422727269999996</v>
       </c>
-      <c r="F99">
+      <c r="G99">
         <v>85.527272730000007</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>47</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="1">
+        <v>98</v>
+      </c>
+      <c r="C100">
         <v>18</v>
       </c>
-      <c r="C100">
-        <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
       <c r="D100">
+        <f t="shared" si="1"/>
+        <v>163</v>
+      </c>
+      <c r="E100">
         <v>5.4738461540000003</v>
       </c>
-      <c r="E100">
+      <c r="F100">
         <v>59.47538462</v>
       </c>
-      <c r="F100">
+      <c r="G100">
         <v>64.94923077</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>31</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="1">
+        <v>99</v>
+      </c>
+      <c r="C101">
         <v>11</v>
       </c>
-      <c r="C101">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
       <c r="D101">
+        <f t="shared" si="1"/>
+        <v>141</v>
+      </c>
+      <c r="E101">
         <v>7.8309523810000004</v>
       </c>
-      <c r="E101">
+      <c r="F101">
         <v>55.823809519999998</v>
       </c>
-      <c r="F101">
+      <c r="G101">
         <v>63.654761899999997</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>33</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="1">
+        <v>100</v>
+      </c>
+      <c r="C102">
         <v>13</v>
       </c>
-      <c r="C102">
-        <f t="shared" si="1"/>
-        <v>46</v>
-      </c>
       <c r="D102">
+        <f t="shared" si="1"/>
+        <v>146</v>
+      </c>
+      <c r="E102">
         <v>6.9804347829999998</v>
       </c>
-      <c r="E102">
+      <c r="F102">
         <v>67.082608699999994</v>
       </c>
-      <c r="F102">
+      <c r="G102">
         <v>74.063043480000005</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>48</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="1">
+        <v>101</v>
+      </c>
+      <c r="C103">
         <v>7</v>
       </c>
-      <c r="C103">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
       <c r="D103">
+        <f t="shared" si="1"/>
+        <v>156</v>
+      </c>
+      <c r="E103">
         <v>10.57454545</v>
       </c>
-      <c r="E103">
+      <c r="F103">
         <v>69.425454549999998</v>
       </c>
-      <c r="F103">
+      <c r="G103">
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>33</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="1">
+        <v>102</v>
+      </c>
+      <c r="C104">
         <v>14</v>
       </c>
-      <c r="C104">
-        <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
       <c r="D104">
+        <f t="shared" si="1"/>
+        <v>149</v>
+      </c>
+      <c r="E104">
         <v>5.5</v>
       </c>
-      <c r="E104">
+      <c r="F104">
         <v>73.461702130000006</v>
       </c>
-      <c r="F104">
+      <c r="G104">
         <v>78.961702130000006</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>20</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="1">
+        <v>103</v>
+      </c>
+      <c r="C105">
         <v>10</v>
       </c>
-      <c r="C105">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
       <c r="D105">
+        <f t="shared" si="1"/>
+        <v>133</v>
+      </c>
+      <c r="E105">
         <v>8.4499999999999993</v>
       </c>
-      <c r="E105">
+      <c r="F105">
         <v>45.97666667</v>
       </c>
-      <c r="F105">
+      <c r="G105">
         <v>54.426666670000003</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
operational data checking trough OracleAssesment class. Now check includes when, while & expressions
</commit_message>
<xml_diff>
--- a/org.xtext.example.Adeptness/resources/TrainingData_MiercolesSur_trainingdata1.xlsx
+++ b/org.xtext.example.Adeptness/resources/TrainingData_MiercolesSur_trainingdata1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\AdeptnessDSL\org.xtext.example.Adeptness\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04302B24-194F-4E50-8B69-9938B880660D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E14937-52AB-4221-B529-10F5D60852F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27720" yWindow="1080" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -376,26 +376,26 @@
   <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="10.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -407,19 +407,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
+        <f>SUM(A2:B2)</f>
+        <v>6</v>
+      </c>
+      <c r="D2" s="1">
         <v>0</v>
-      </c>
-      <c r="D2">
-        <f>SUM(A2:C2)</f>
-        <v>6</v>
       </c>
       <c r="E2">
         <v>3.3333333329999999E-2</v>
@@ -431,19 +431,19 @@
         <v>57.483333330000001</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>SUM(A3:B3)</f>
+        <v>6</v>
+      </c>
+      <c r="D3" s="1">
         <v>1</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D66" si="0">SUM(A3:C3)</f>
-        <v>7</v>
       </c>
       <c r="E3">
         <v>3.1</v>
@@ -455,19 +455,19 @@
         <v>43.483333330000001</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>8</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f>SUM(A4:B4)</f>
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
         <v>2.5</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>11.5</v>
       </c>
       <c r="E4">
         <v>5.4</v>
@@ -479,19 +479,19 @@
         <v>46.044444439999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>7</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f>SUM(A5:B5)</f>
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
         <v>3</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>10</v>
       </c>
       <c r="E5">
         <v>10.84285714</v>
@@ -503,19 +503,19 @@
         <v>70.571428569999995</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>8</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f>SUM(A6:B6)</f>
+        <v>8</v>
+      </c>
+      <c r="D6" s="1">
         <v>4</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>12</v>
       </c>
       <c r="E6">
         <v>15.025</v>
@@ -527,19 +527,19 @@
         <v>67.650000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>10</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f>SUM(A7:B7)</f>
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
         <v>5</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>15</v>
       </c>
       <c r="E7">
         <v>10.9</v>
@@ -551,19 +551,19 @@
         <v>74.2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f>SUM(A8:B8)</f>
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
         <v>6.5</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>12.5</v>
       </c>
       <c r="E8">
         <v>17.43333333</v>
@@ -575,19 +575,19 @@
         <v>61.55</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f>SUM(A9:B9)</f>
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
         <v>7.5</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>17.5</v>
       </c>
       <c r="E9">
         <v>11.46</v>
@@ -599,19 +599,19 @@
         <v>61.18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f>SUM(A10:B10)</f>
+        <v>10</v>
+      </c>
+      <c r="D10" s="1">
         <v>8</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>18</v>
       </c>
       <c r="E10">
         <v>13.3</v>
@@ -623,19 +623,19 @@
         <v>66.94</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>14</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f>SUM(A11:B11)</f>
+        <v>14</v>
+      </c>
+      <c r="D11" s="1">
         <v>8.99</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>22.990000000000002</v>
       </c>
       <c r="E11">
         <v>9.9285714289999998</v>
@@ -647,19 +647,19 @@
         <v>71.142857140000004</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>13</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <f>SUM(A12:B12)</f>
+        <v>17</v>
+      </c>
+      <c r="D12" s="1">
         <v>9.5</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>26.5</v>
       </c>
       <c r="E12">
         <v>9.1705882350000003</v>
@@ -671,19 +671,19 @@
         <v>77.92352941</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>18</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <f>SUM(A13:B13)</f>
+        <v>20</v>
+      </c>
+      <c r="D13" s="1">
         <v>10.89</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>30.89</v>
       </c>
       <c r="E13">
         <v>10.14</v>
@@ -695,19 +695,19 @@
         <v>63.185000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>18</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f>SUM(A14:B14)</f>
+        <v>19</v>
+      </c>
+      <c r="D14" s="1">
         <v>12</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>31</v>
       </c>
       <c r="E14">
         <v>6.268421053</v>
@@ -719,19 +719,19 @@
         <v>96.984210529999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>23</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f>SUM(A15:B15)</f>
+        <v>23</v>
+      </c>
+      <c r="D15" s="1">
         <v>13</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>36</v>
       </c>
       <c r="E15">
         <v>8.8913043480000002</v>
@@ -743,19 +743,19 @@
         <v>91.96086957</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>25</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <f>SUM(A16:B16)</f>
+        <v>30</v>
+      </c>
+      <c r="D16" s="1">
         <v>14</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>44</v>
       </c>
       <c r="E16">
         <v>7.4766666669999999</v>
@@ -767,19 +767,19 @@
         <v>75.05</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>29</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <f>SUM(A17:B17)</f>
+        <v>31</v>
+      </c>
+      <c r="D17" s="1">
         <v>14.8</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>45.8</v>
       </c>
       <c r="E17">
         <v>7.0354838710000003</v>
@@ -791,19 +791,19 @@
         <v>91.132258059999998</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>26</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <f>SUM(A18:B18)</f>
+        <v>30</v>
+      </c>
+      <c r="D18" s="1">
         <v>15.86</v>
-      </c>
-      <c r="C18">
-        <v>4</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>45.86</v>
       </c>
       <c r="E18">
         <v>10.50666667</v>
@@ -815,19 +815,19 @@
         <v>73.16</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>25</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <f>SUM(A19:B19)</f>
+        <v>27</v>
+      </c>
+      <c r="D19" s="1">
         <v>17</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>44</v>
       </c>
       <c r="E19">
         <v>12.996296299999999</v>
@@ -839,19 +839,19 @@
         <v>69.385185190000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>33</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <f>SUM(A20:B20)</f>
+        <v>34</v>
+      </c>
+      <c r="D20" s="1">
         <v>18</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>52</v>
       </c>
       <c r="E20">
         <v>10.60882353</v>
@@ -863,19 +863,19 @@
         <v>91.573529410000006</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>38</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <f>SUM(A21:B21)</f>
+        <v>41</v>
+      </c>
+      <c r="D21" s="1">
         <v>18.899999999999999</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>59.9</v>
       </c>
       <c r="E21">
         <v>3.7439024390000002</v>
@@ -887,19 +887,19 @@
         <v>92.897560979999994</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>30</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <f>SUM(A22:B22)</f>
+        <v>35</v>
+      </c>
+      <c r="D22" s="1">
         <v>20</v>
-      </c>
-      <c r="C22">
-        <v>5</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>55</v>
       </c>
       <c r="E22">
         <v>9.5628571430000004</v>
@@ -911,19 +911,19 @@
         <v>77.58</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>25</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <f>SUM(A23:B23)</f>
+        <v>29</v>
+      </c>
+      <c r="D23" s="1">
         <v>21</v>
-      </c>
-      <c r="C23">
-        <v>4</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>50</v>
       </c>
       <c r="E23">
         <v>7.5793103449999997</v>
@@ -935,19 +935,19 @@
         <v>69.993103450000007</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>38</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <f>SUM(A24:B24)</f>
+        <v>43</v>
+      </c>
+      <c r="D24" s="1">
         <v>22</v>
-      </c>
-      <c r="C24">
-        <v>5</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>65</v>
       </c>
       <c r="E24">
         <v>8.0581395350000005</v>
@@ -959,19 +959,19 @@
         <v>92.844186050000005</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>40</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <f>SUM(A25:B25)</f>
+        <v>44</v>
+      </c>
+      <c r="D25" s="1">
         <v>23</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>67</v>
       </c>
       <c r="E25">
         <v>6.4295454550000004</v>
@@ -983,19 +983,19 @@
         <v>82.109090910000006</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>40</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <f>SUM(A26:B26)</f>
+        <v>45</v>
+      </c>
+      <c r="D26" s="1">
         <v>24</v>
-      </c>
-      <c r="C26">
-        <v>5</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>69</v>
       </c>
       <c r="E26">
         <v>7.448888889</v>
@@ -1007,19 +1007,19 @@
         <v>93.657777780000004</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>59</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <f>SUM(A27:B27)</f>
+        <v>69</v>
+      </c>
+      <c r="D27" s="1">
         <v>25</v>
-      </c>
-      <c r="C27">
-        <v>10</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>94</v>
       </c>
       <c r="E27">
         <v>6.7927536230000003</v>
@@ -1031,19 +1031,19 @@
         <v>113.9115942</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>44</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <f>SUM(A28:B28)</f>
+        <v>47</v>
+      </c>
+      <c r="D28" s="1">
         <v>26</v>
-      </c>
-      <c r="C28">
-        <v>3</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
-        <v>73</v>
       </c>
       <c r="E28">
         <v>6.2361702130000003</v>
@@ -1055,19 +1055,19 @@
         <v>113.46595739999999</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>47</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <f>SUM(A29:B29)</f>
+        <v>51</v>
+      </c>
+      <c r="D29" s="1">
         <v>27</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="0"/>
-        <v>78</v>
       </c>
       <c r="E29">
         <v>7.1666666670000003</v>
@@ -1079,19 +1079,19 @@
         <v>89.627450980000006</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>44</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <f>SUM(A30:B30)</f>
+        <v>55</v>
+      </c>
+      <c r="D30" s="1">
         <v>28</v>
-      </c>
-      <c r="C30">
-        <v>11</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="0"/>
-        <v>83</v>
       </c>
       <c r="E30">
         <v>7.1890909089999999</v>
@@ -1103,19 +1103,19 @@
         <v>88.598181819999994</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>59</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <f>SUM(A31:B31)</f>
+        <v>69</v>
+      </c>
+      <c r="D31" s="1">
         <v>29</v>
-      </c>
-      <c r="C31">
-        <v>10</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="0"/>
-        <v>98</v>
       </c>
       <c r="E31">
         <v>7.5333333329999999</v>
@@ -1127,19 +1127,19 @@
         <v>101.1304348</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>46</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <f>SUM(A32:B32)</f>
+        <v>57</v>
+      </c>
+      <c r="D32" s="1">
         <v>30</v>
-      </c>
-      <c r="C32">
-        <v>11</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="0"/>
-        <v>87</v>
       </c>
       <c r="E32">
         <v>9.1859649119999993</v>
@@ -1151,19 +1151,19 @@
         <v>89.331578949999994</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>42</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33">
+        <v>12</v>
+      </c>
+      <c r="C33">
+        <f>SUM(A33:B33)</f>
+        <v>54</v>
+      </c>
+      <c r="D33" s="1">
         <v>31</v>
-      </c>
-      <c r="C33">
-        <v>12</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="0"/>
-        <v>85</v>
       </c>
       <c r="E33">
         <v>7.9537037039999996</v>
@@ -1175,19 +1175,19 @@
         <v>82.916666669999998</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>56</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34">
+        <v>14</v>
+      </c>
+      <c r="C34">
+        <f>SUM(A34:B34)</f>
+        <v>70</v>
+      </c>
+      <c r="D34" s="1">
         <v>32</v>
-      </c>
-      <c r="C34">
-        <v>14</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="0"/>
-        <v>102</v>
       </c>
       <c r="E34">
         <v>7.6385714289999997</v>
@@ -1199,19 +1199,19 @@
         <v>95.05285714</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>41</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <f>SUM(A35:B35)</f>
+        <v>52</v>
+      </c>
+      <c r="D35" s="1">
         <v>33</v>
-      </c>
-      <c r="C35">
-        <v>11</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="0"/>
-        <v>85</v>
       </c>
       <c r="E35">
         <v>7.5461538460000002</v>
@@ -1223,19 +1223,19 @@
         <v>83.136538459999997</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>39</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <f>SUM(A36:B36)</f>
+        <v>50</v>
+      </c>
+      <c r="D36" s="1">
         <v>34</v>
-      </c>
-      <c r="C36">
-        <v>11</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="0"/>
-        <v>84</v>
       </c>
       <c r="E36">
         <v>2.3959999999999999</v>
@@ -1247,19 +1247,19 @@
         <v>89.278000000000006</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>53</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37">
+        <v>20</v>
+      </c>
+      <c r="C37">
+        <f>SUM(A37:B37)</f>
+        <v>73</v>
+      </c>
+      <c r="D37" s="1">
         <v>35</v>
-      </c>
-      <c r="C37">
-        <v>20</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="0"/>
-        <v>108</v>
       </c>
       <c r="E37">
         <v>8.9917808220000008</v>
@@ -1271,19 +1271,19 @@
         <v>84.006849320000001</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>39</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38">
+        <v>16</v>
+      </c>
+      <c r="C38">
+        <f>SUM(A38:B38)</f>
+        <v>55</v>
+      </c>
+      <c r="D38" s="1">
         <v>36</v>
-      </c>
-      <c r="C38">
-        <v>16</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="0"/>
-        <v>91</v>
       </c>
       <c r="E38">
         <v>12.06</v>
@@ -1295,19 +1295,19 @@
         <v>74.43090909</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39">
+        <v>15</v>
+      </c>
+      <c r="C39">
+        <f>SUM(A39:B39)</f>
+        <v>53</v>
+      </c>
+      <c r="D39" s="1">
         <v>37</v>
-      </c>
-      <c r="C39">
-        <v>15</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="0"/>
-        <v>90</v>
       </c>
       <c r="E39">
         <v>6.5943396229999998</v>
@@ -1319,19 +1319,19 @@
         <v>65.969811320000005</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40">
+        <v>16</v>
+      </c>
+      <c r="C40">
+        <f>SUM(A40:B40)</f>
+        <v>54</v>
+      </c>
+      <c r="D40" s="1">
         <v>38</v>
-      </c>
-      <c r="C40">
-        <v>16</v>
-      </c>
-      <c r="D40">
-        <f t="shared" si="0"/>
-        <v>92</v>
       </c>
       <c r="E40">
         <v>8.6703703700000005</v>
@@ -1343,19 +1343,19 @@
         <v>65.622222219999998</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>21</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <f>SUM(A41:B41)</f>
+        <v>35</v>
+      </c>
+      <c r="D41" s="1">
         <v>39</v>
-      </c>
-      <c r="C41">
-        <v>14</v>
-      </c>
-      <c r="D41">
-        <f t="shared" si="0"/>
-        <v>74</v>
       </c>
       <c r="E41">
         <v>4.1028571429999996</v>
@@ -1367,19 +1367,19 @@
         <v>66.16857143</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>24</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <f>SUM(A42:B42)</f>
+        <v>34</v>
+      </c>
+      <c r="D42" s="1">
         <v>40</v>
-      </c>
-      <c r="C42">
-        <v>10</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="0"/>
-        <v>74</v>
       </c>
       <c r="E42">
         <v>12.08529412</v>
@@ -1391,19 +1391,19 @@
         <v>65.667647059999993</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>32</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43">
+        <v>17</v>
+      </c>
+      <c r="C43">
+        <f>SUM(A43:B43)</f>
+        <v>49</v>
+      </c>
+      <c r="D43" s="1">
         <v>41</v>
-      </c>
-      <c r="C43">
-        <v>17</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="0"/>
-        <v>90</v>
       </c>
       <c r="E43">
         <v>8.1857142859999996</v>
@@ -1415,19 +1415,19 @@
         <v>56.053061219999996</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>23</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44">
+        <v>13</v>
+      </c>
+      <c r="C44">
+        <f>SUM(A44:B44)</f>
+        <v>36</v>
+      </c>
+      <c r="D44" s="1">
         <v>42</v>
-      </c>
-      <c r="C44">
-        <v>13</v>
-      </c>
-      <c r="D44">
-        <f t="shared" si="0"/>
-        <v>78</v>
       </c>
       <c r="E44">
         <v>10.89722222</v>
@@ -1439,19 +1439,19 @@
         <v>67.916666669999998</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>24</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45">
+        <v>17</v>
+      </c>
+      <c r="C45">
+        <f>SUM(A45:B45)</f>
+        <v>41</v>
+      </c>
+      <c r="D45" s="1">
         <v>43</v>
-      </c>
-      <c r="C45">
-        <v>17</v>
-      </c>
-      <c r="D45">
-        <f t="shared" si="0"/>
-        <v>84</v>
       </c>
       <c r="E45">
         <v>6.1780487800000001</v>
@@ -1463,19 +1463,19 @@
         <v>54.1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>28</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46">
+        <v>16</v>
+      </c>
+      <c r="C46">
+        <f>SUM(A46:B46)</f>
         <v>44</v>
       </c>
-      <c r="C46">
-        <v>16</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="0"/>
-        <v>88</v>
+      <c r="D46" s="1">
+        <v>44</v>
       </c>
       <c r="E46">
         <v>4.7659090910000002</v>
@@ -1487,19 +1487,19 @@
         <v>64.963636359999995</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>10</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47">
+        <v>19</v>
+      </c>
+      <c r="C47">
+        <f>SUM(A47:B47)</f>
+        <v>29</v>
+      </c>
+      <c r="D47" s="1">
         <v>45</v>
-      </c>
-      <c r="C47">
-        <v>19</v>
-      </c>
-      <c r="D47">
-        <f t="shared" si="0"/>
-        <v>74</v>
       </c>
       <c r="E47">
         <v>6.6793103450000002</v>
@@ -1511,19 +1511,19 @@
         <v>46.25517241</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>27</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48">
+        <v>24</v>
+      </c>
+      <c r="C48">
+        <f>SUM(A48:B48)</f>
+        <v>51</v>
+      </c>
+      <c r="D48" s="1">
         <v>46</v>
-      </c>
-      <c r="C48">
-        <v>24</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="0"/>
-        <v>97</v>
       </c>
       <c r="E48">
         <v>10.50784314</v>
@@ -1535,19 +1535,19 @@
         <v>54.523529410000002</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>24</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49">
+        <v>36</v>
+      </c>
+      <c r="C49">
+        <f>SUM(A49:B49)</f>
+        <v>60</v>
+      </c>
+      <c r="D49" s="1">
         <v>47</v>
-      </c>
-      <c r="C49">
-        <v>36</v>
-      </c>
-      <c r="D49">
-        <f t="shared" si="0"/>
-        <v>107</v>
       </c>
       <c r="E49">
         <v>13.855</v>
@@ -1559,19 +1559,19 @@
         <v>67.709999999999994</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>28</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50">
+        <v>14</v>
+      </c>
+      <c r="C50">
+        <f>SUM(A50:B50)</f>
+        <v>42</v>
+      </c>
+      <c r="D50" s="1">
         <v>48</v>
-      </c>
-      <c r="C50">
-        <v>14</v>
-      </c>
-      <c r="D50">
-        <f t="shared" si="0"/>
-        <v>90</v>
       </c>
       <c r="E50">
         <v>8.7714285709999995</v>
@@ -1583,19 +1583,19 @@
         <v>77.209523809999993</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>27</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51">
+        <v>24</v>
+      </c>
+      <c r="C51">
+        <f>SUM(A51:B51)</f>
+        <v>51</v>
+      </c>
+      <c r="D51" s="1">
         <v>49</v>
-      </c>
-      <c r="C51">
-        <v>24</v>
-      </c>
-      <c r="D51">
-        <f t="shared" si="0"/>
-        <v>100</v>
       </c>
       <c r="E51">
         <v>11.176470589999999</v>
@@ -1607,19 +1607,19 @@
         <v>64.372549019999994</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>27</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52">
+        <v>28</v>
+      </c>
+      <c r="C52">
+        <f>SUM(A52:B52)</f>
+        <v>55</v>
+      </c>
+      <c r="D52" s="1">
         <v>50</v>
-      </c>
-      <c r="C52">
-        <v>28</v>
-      </c>
-      <c r="D52">
-        <f t="shared" si="0"/>
-        <v>105</v>
       </c>
       <c r="E52">
         <v>15.38545455</v>
@@ -1631,19 +1631,19 @@
         <v>82.532727269999995</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>18</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53">
+        <v>26</v>
+      </c>
+      <c r="C53">
+        <f>SUM(A53:B53)</f>
+        <v>44</v>
+      </c>
+      <c r="D53" s="1">
         <v>51</v>
-      </c>
-      <c r="C53">
-        <v>26</v>
-      </c>
-      <c r="D53">
-        <f t="shared" si="0"/>
-        <v>95</v>
       </c>
       <c r="E53">
         <v>6.8772727270000003</v>
@@ -1655,19 +1655,19 @@
         <v>58.465909089999997</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>14</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54">
+        <v>13</v>
+      </c>
+      <c r="C54">
+        <f>SUM(A54:B54)</f>
+        <v>27</v>
+      </c>
+      <c r="D54" s="1">
         <v>52</v>
-      </c>
-      <c r="C54">
-        <v>13</v>
-      </c>
-      <c r="D54">
-        <f t="shared" si="0"/>
-        <v>79</v>
       </c>
       <c r="E54">
         <v>6.5037037040000003</v>
@@ -1679,19 +1679,19 @@
         <v>55.611111110000003</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>23</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55">
+        <v>18</v>
+      </c>
+      <c r="C55">
+        <f>SUM(A55:B55)</f>
+        <v>41</v>
+      </c>
+      <c r="D55" s="1">
         <v>53</v>
-      </c>
-      <c r="C55">
-        <v>18</v>
-      </c>
-      <c r="D55">
-        <f t="shared" si="0"/>
-        <v>94</v>
       </c>
       <c r="E55">
         <v>6.456097561</v>
@@ -1703,19 +1703,19 @@
         <v>65.041463410000006</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>25</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56">
+        <v>17</v>
+      </c>
+      <c r="C56">
+        <f>SUM(A56:B56)</f>
+        <v>42</v>
+      </c>
+      <c r="D56" s="1">
         <v>54</v>
-      </c>
-      <c r="C56">
-        <v>17</v>
-      </c>
-      <c r="D56">
-        <f t="shared" si="0"/>
-        <v>96</v>
       </c>
       <c r="E56">
         <v>5.845238095</v>
@@ -1727,19 +1727,19 @@
         <v>56.580952379999999</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>21</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57">
+        <v>17</v>
+      </c>
+      <c r="C57">
+        <f>SUM(A57:B57)</f>
+        <v>38</v>
+      </c>
+      <c r="D57" s="1">
         <v>55</v>
-      </c>
-      <c r="C57">
-        <v>17</v>
-      </c>
-      <c r="D57">
-        <f t="shared" si="0"/>
-        <v>93</v>
       </c>
       <c r="E57">
         <v>7.3421052629999997</v>
@@ -1751,19 +1751,19 @@
         <v>52.05</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>31</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58">
+        <v>12</v>
+      </c>
+      <c r="C58">
+        <f>SUM(A58:B58)</f>
+        <v>43</v>
+      </c>
+      <c r="D58" s="1">
         <v>56</v>
-      </c>
-      <c r="C58">
-        <v>12</v>
-      </c>
-      <c r="D58">
-        <f t="shared" si="0"/>
-        <v>99</v>
       </c>
       <c r="E58">
         <v>5.0418604650000001</v>
@@ -1775,19 +1775,19 @@
         <v>60.511627910000001</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>11</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59">
+        <v>9</v>
+      </c>
+      <c r="C59">
+        <f>SUM(A59:B59)</f>
+        <v>20</v>
+      </c>
+      <c r="D59" s="1">
         <v>57</v>
-      </c>
-      <c r="C59">
-        <v>9</v>
-      </c>
-      <c r="D59">
-        <f t="shared" si="0"/>
-        <v>77</v>
       </c>
       <c r="E59">
         <v>6.2949999999999999</v>
@@ -1799,19 +1799,19 @@
         <v>50.7</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>23</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60">
+        <v>20</v>
+      </c>
+      <c r="C60">
+        <f>SUM(A60:B60)</f>
+        <v>43</v>
+      </c>
+      <c r="D60" s="1">
         <v>58</v>
-      </c>
-      <c r="C60">
-        <v>20</v>
-      </c>
-      <c r="D60">
-        <f t="shared" si="0"/>
-        <v>101</v>
       </c>
       <c r="E60">
         <v>7.3930232560000002</v>
@@ -1823,19 +1823,19 @@
         <v>55.68372093</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>26</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61">
+        <v>20</v>
+      </c>
+      <c r="C61">
+        <f>SUM(A61:B61)</f>
+        <v>46</v>
+      </c>
+      <c r="D61" s="1">
         <v>59</v>
-      </c>
-      <c r="C61">
-        <v>20</v>
-      </c>
-      <c r="D61">
-        <f t="shared" si="0"/>
-        <v>105</v>
       </c>
       <c r="E61">
         <v>12.72173913</v>
@@ -1847,19 +1847,19 @@
         <v>61.867391300000001</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>30</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62">
+        <v>35</v>
+      </c>
+      <c r="C62">
+        <f>SUM(A62:B62)</f>
+        <v>65</v>
+      </c>
+      <c r="D62" s="1">
         <v>60</v>
-      </c>
-      <c r="C62">
-        <v>35</v>
-      </c>
-      <c r="D62">
-        <f t="shared" si="0"/>
-        <v>125</v>
       </c>
       <c r="E62">
         <v>15.74</v>
@@ -1871,19 +1871,19 @@
         <v>67.066153850000006</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>32</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63">
+        <v>20</v>
+      </c>
+      <c r="C63">
+        <f>SUM(A63:B63)</f>
+        <v>52</v>
+      </c>
+      <c r="D63" s="1">
         <v>61</v>
-      </c>
-      <c r="C63">
-        <v>20</v>
-      </c>
-      <c r="D63">
-        <f t="shared" si="0"/>
-        <v>113</v>
       </c>
       <c r="E63">
         <v>16.265384619999999</v>
@@ -1895,19 +1895,19 @@
         <v>70.105769230000007</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>28</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64">
+        <v>7</v>
+      </c>
+      <c r="C64">
+        <f>SUM(A64:B64)</f>
+        <v>35</v>
+      </c>
+      <c r="D64" s="1">
         <v>62</v>
-      </c>
-      <c r="C64">
-        <v>7</v>
-      </c>
-      <c r="D64">
-        <f t="shared" si="0"/>
-        <v>97</v>
       </c>
       <c r="E64">
         <v>5.9942857140000001</v>
@@ -1919,19 +1919,19 @@
         <v>51.737142859999999</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>26</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65">
+        <v>19</v>
+      </c>
+      <c r="C65">
+        <f>SUM(A65:B65)</f>
+        <v>45</v>
+      </c>
+      <c r="D65" s="1">
         <v>63</v>
-      </c>
-      <c r="C65">
-        <v>19</v>
-      </c>
-      <c r="D65">
-        <f t="shared" si="0"/>
-        <v>108</v>
       </c>
       <c r="E65">
         <v>7.6111111109999996</v>
@@ -1943,19 +1943,19 @@
         <v>51.82222222</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>22</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66">
+        <v>23</v>
+      </c>
+      <c r="C66">
+        <f>SUM(A66:B66)</f>
+        <v>45</v>
+      </c>
+      <c r="D66" s="1">
         <v>64</v>
-      </c>
-      <c r="C66">
-        <v>23</v>
-      </c>
-      <c r="D66">
-        <f t="shared" si="0"/>
-        <v>109</v>
       </c>
       <c r="E66">
         <v>7.7777777779999999</v>
@@ -1967,19 +1967,19 @@
         <v>58.455555560000001</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>8</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67">
+        <v>13</v>
+      </c>
+      <c r="C67">
+        <f t="shared" ref="C67:C105" si="0">SUM(A67:B67)</f>
+        <v>21</v>
+      </c>
+      <c r="D67" s="1">
         <v>65</v>
-      </c>
-      <c r="C67">
-        <v>13</v>
-      </c>
-      <c r="D67">
-        <f t="shared" ref="D67:D105" si="1">SUM(A67:C67)</f>
-        <v>86</v>
       </c>
       <c r="E67">
         <v>7.9857142860000003</v>
@@ -1991,19 +1991,19 @@
         <v>48.985714289999997</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>13</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68">
+        <v>13</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D68" s="1">
         <v>66</v>
-      </c>
-      <c r="C68">
-        <v>13</v>
-      </c>
-      <c r="D68">
-        <f t="shared" si="1"/>
-        <v>92</v>
       </c>
       <c r="E68">
         <v>9.3730769229999993</v>
@@ -2015,19 +2015,19 @@
         <v>52.157692310000002</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>23</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69">
+        <v>8</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D69" s="1">
         <v>67</v>
-      </c>
-      <c r="C69">
-        <v>8</v>
-      </c>
-      <c r="D69">
-        <f t="shared" si="1"/>
-        <v>98</v>
       </c>
       <c r="E69">
         <v>8.3677419349999997</v>
@@ -2039,19 +2039,19 @@
         <v>55.603225809999998</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>14</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70">
+        <v>25</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D70" s="1">
         <v>68</v>
-      </c>
-      <c r="C70">
-        <v>25</v>
-      </c>
-      <c r="D70">
-        <f t="shared" si="1"/>
-        <v>107</v>
       </c>
       <c r="E70">
         <v>8.4128205129999998</v>
@@ -2063,19 +2063,19 @@
         <v>64.851282049999995</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>8</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71">
+        <v>14</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D71" s="1">
         <v>69</v>
-      </c>
-      <c r="C71">
-        <v>14</v>
-      </c>
-      <c r="D71">
-        <f t="shared" si="1"/>
-        <v>91</v>
       </c>
       <c r="E71">
         <v>8.5545454549999995</v>
@@ -2087,19 +2087,19 @@
         <v>64.363636360000001</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>12</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72">
+        <v>6</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D72" s="1">
         <v>70</v>
-      </c>
-      <c r="C72">
-        <v>6</v>
-      </c>
-      <c r="D72">
-        <f t="shared" si="1"/>
-        <v>88</v>
       </c>
       <c r="E72">
         <v>4.7777777779999999</v>
@@ -2111,19 +2111,19 @@
         <v>46.022222220000003</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>14</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73">
+        <v>20</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D73" s="1">
         <v>71</v>
-      </c>
-      <c r="C73">
-        <v>20</v>
-      </c>
-      <c r="D73">
-        <f t="shared" si="1"/>
-        <v>105</v>
       </c>
       <c r="E73">
         <v>8.3705882349999996</v>
@@ -2135,19 +2135,19 @@
         <v>59.232352939999998</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>20</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74">
+        <v>37</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="D74" s="1">
         <v>72</v>
-      </c>
-      <c r="C74">
-        <v>37</v>
-      </c>
-      <c r="D74">
-        <f t="shared" si="1"/>
-        <v>129</v>
       </c>
       <c r="E74">
         <v>9.5964912279999997</v>
@@ -2159,19 +2159,19 @@
         <v>68.064912280000001</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>16</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75">
+        <v>45</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="D75" s="1">
         <v>73</v>
-      </c>
-      <c r="C75">
-        <v>45</v>
-      </c>
-      <c r="D75">
-        <f t="shared" si="1"/>
-        <v>134</v>
       </c>
       <c r="E75">
         <v>11.244262300000001</v>
@@ -2183,19 +2183,19 @@
         <v>74.572131150000004</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>15</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76">
+        <v>30</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D76" s="1">
         <v>74</v>
-      </c>
-      <c r="C76">
-        <v>30</v>
-      </c>
-      <c r="D76">
-        <f t="shared" si="1"/>
-        <v>119</v>
       </c>
       <c r="E76">
         <v>7.6466666669999999</v>
@@ -2207,19 +2207,19 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>21</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77">
+        <v>41</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="D77" s="1">
         <v>75</v>
-      </c>
-      <c r="C77">
-        <v>41</v>
-      </c>
-      <c r="D77">
-        <f t="shared" si="1"/>
-        <v>137</v>
       </c>
       <c r="E77">
         <v>8.2225806450000007</v>
@@ -2231,19 +2231,19 @@
         <v>67.301612899999995</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>8</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78">
+        <v>33</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D78" s="1">
         <v>76</v>
-      </c>
-      <c r="C78">
-        <v>33</v>
-      </c>
-      <c r="D78">
-        <f t="shared" si="1"/>
-        <v>117</v>
       </c>
       <c r="E78">
         <v>12.70731707</v>
@@ -2255,19 +2255,19 @@
         <v>63.897560980000002</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>10</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79">
+        <v>43</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="D79" s="1">
         <v>77</v>
-      </c>
-      <c r="C79">
-        <v>43</v>
-      </c>
-      <c r="D79">
-        <f t="shared" si="1"/>
-        <v>130</v>
       </c>
       <c r="E79">
         <v>13.50754717</v>
@@ -2279,19 +2279,19 @@
         <v>60.354716979999999</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>16</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80">
+        <v>35</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="D80" s="1">
         <v>78</v>
-      </c>
-      <c r="C80">
-        <v>35</v>
-      </c>
-      <c r="D80">
-        <f t="shared" si="1"/>
-        <v>129</v>
       </c>
       <c r="E80">
         <v>7.2764705879999996</v>
@@ -2303,19 +2303,19 @@
         <v>55.913725489999997</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>19</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81">
+        <v>28</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D81" s="1">
         <v>79</v>
-      </c>
-      <c r="C81">
-        <v>28</v>
-      </c>
-      <c r="D81">
-        <f t="shared" si="1"/>
-        <v>126</v>
       </c>
       <c r="E81">
         <v>8.9723404260000006</v>
@@ -2327,19 +2327,19 @@
         <v>58.861702129999998</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>19</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82">
+        <v>33</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="D82" s="1">
         <v>80</v>
-      </c>
-      <c r="C82">
-        <v>33</v>
-      </c>
-      <c r="D82">
-        <f t="shared" si="1"/>
-        <v>132</v>
       </c>
       <c r="E82">
         <v>11.16923077</v>
@@ -2351,19 +2351,19 @@
         <v>61.146153849999997</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>12</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83">
+        <v>51</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="D83" s="1">
         <v>81</v>
-      </c>
-      <c r="C83">
-        <v>51</v>
-      </c>
-      <c r="D83">
-        <f t="shared" si="1"/>
-        <v>144</v>
       </c>
       <c r="E83">
         <v>14.21587302</v>
@@ -2375,19 +2375,19 @@
         <v>60.882539680000001</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>18</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84">
+        <v>18</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D84" s="1">
         <v>82</v>
-      </c>
-      <c r="C84">
-        <v>18</v>
-      </c>
-      <c r="D84">
-        <f t="shared" si="1"/>
-        <v>118</v>
       </c>
       <c r="E84">
         <v>9.5749999999999993</v>
@@ -2399,19 +2399,19 @@
         <v>55.013888889999997</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>19</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85">
+        <v>26</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D85" s="1">
         <v>83</v>
-      </c>
-      <c r="C85">
-        <v>26</v>
-      </c>
-      <c r="D85">
-        <f t="shared" si="1"/>
-        <v>128</v>
       </c>
       <c r="E85">
         <v>10.50222222</v>
@@ -2423,19 +2423,19 @@
         <v>60.77333333</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>35</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86">
+        <v>58</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="D86" s="1">
         <v>84</v>
-      </c>
-      <c r="C86">
-        <v>58</v>
-      </c>
-      <c r="D86">
-        <f t="shared" si="1"/>
-        <v>177</v>
       </c>
       <c r="E86">
         <v>9.2440860219999994</v>
@@ -2447,19 +2447,19 @@
         <v>64.358064519999999</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>32</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87">
+        <v>49</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="D87" s="1">
         <v>85</v>
-      </c>
-      <c r="C87">
-        <v>49</v>
-      </c>
-      <c r="D87">
-        <f t="shared" si="1"/>
-        <v>166</v>
       </c>
       <c r="E87">
         <v>10.08024691</v>
@@ -2471,19 +2471,19 @@
         <v>67.758024689999999</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>31</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88">
+        <v>43</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="D88" s="1">
         <v>86</v>
-      </c>
-      <c r="C88">
-        <v>43</v>
-      </c>
-      <c r="D88">
-        <f t="shared" si="1"/>
-        <v>160</v>
       </c>
       <c r="E88">
         <v>13.917567569999999</v>
@@ -2495,19 +2495,19 @@
         <v>86.524324320000005</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>60</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89">
+        <v>44</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="D89" s="1">
         <v>87</v>
-      </c>
-      <c r="C89">
-        <v>44</v>
-      </c>
-      <c r="D89">
-        <f t="shared" si="1"/>
-        <v>191</v>
       </c>
       <c r="E89">
         <v>20.94038462</v>
@@ -2519,19 +2519,19 @@
         <v>94.474038460000003</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>37</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90">
+        <v>23</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="D90" s="1">
         <v>88</v>
-      </c>
-      <c r="C90">
-        <v>23</v>
-      </c>
-      <c r="D90">
-        <f t="shared" si="1"/>
-        <v>148</v>
       </c>
       <c r="E90">
         <v>7.1566666669999996</v>
@@ -2543,19 +2543,19 @@
         <v>62.806666669999998</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>42</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91">
+        <v>21</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="D91" s="1">
         <v>89</v>
-      </c>
-      <c r="C91">
-        <v>21</v>
-      </c>
-      <c r="D91">
-        <f t="shared" si="1"/>
-        <v>152</v>
       </c>
       <c r="E91">
         <v>8.7523809519999993</v>
@@ -2567,19 +2567,19 @@
         <v>70.238095240000007</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>18</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92">
+        <v>24</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D92" s="1">
         <v>90</v>
-      </c>
-      <c r="C92">
-        <v>24</v>
-      </c>
-      <c r="D92">
-        <f t="shared" si="1"/>
-        <v>132</v>
       </c>
       <c r="E92">
         <v>7.7285714289999996</v>
@@ -2591,19 +2591,19 @@
         <v>61.128571430000001</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>15</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93">
+        <v>20</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D93" s="1">
         <v>91</v>
-      </c>
-      <c r="C93">
-        <v>20</v>
-      </c>
-      <c r="D93">
-        <f t="shared" si="1"/>
-        <v>126</v>
       </c>
       <c r="E93">
         <v>6.6371428569999997</v>
@@ -2615,19 +2615,19 @@
         <v>51.01714286</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>21</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94">
+        <v>11</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D94" s="1">
         <v>92</v>
-      </c>
-      <c r="C94">
-        <v>11</v>
-      </c>
-      <c r="D94">
-        <f t="shared" si="1"/>
-        <v>124</v>
       </c>
       <c r="E94">
         <v>4.859375</v>
@@ -2639,19 +2639,19 @@
         <v>58.174999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>23</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95">
+        <v>15</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D95" s="1">
         <v>93</v>
-      </c>
-      <c r="C95">
-        <v>15</v>
-      </c>
-      <c r="D95">
-        <f t="shared" si="1"/>
-        <v>131</v>
       </c>
       <c r="E95">
         <v>8.0657894740000007</v>
@@ -2663,19 +2663,19 @@
         <v>71.281578949999997</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>21</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96">
+        <v>7</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D96" s="1">
         <v>94</v>
-      </c>
-      <c r="C96">
-        <v>7</v>
-      </c>
-      <c r="D96">
-        <f t="shared" si="1"/>
-        <v>122</v>
       </c>
       <c r="E96">
         <v>3.5714285710000002</v>
@@ -2687,19 +2687,19 @@
         <v>61.553571429999998</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>32</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97">
+        <v>19</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="D97" s="1">
         <v>95</v>
-      </c>
-      <c r="C97">
-        <v>19</v>
-      </c>
-      <c r="D97">
-        <f t="shared" si="1"/>
-        <v>146</v>
       </c>
       <c r="E97">
         <v>8.1431372549999992</v>
@@ -2711,19 +2711,19 @@
         <v>72.094117650000001</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>74</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98">
+        <v>39</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="D98" s="1">
         <v>96</v>
-      </c>
-      <c r="C98">
-        <v>39</v>
-      </c>
-      <c r="D98">
-        <f t="shared" si="1"/>
-        <v>209</v>
       </c>
       <c r="E98">
         <v>18.784070799999999</v>
@@ -2735,19 +2735,19 @@
         <v>91.475221239999996</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>47</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99">
+        <v>41</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="D99" s="1">
         <v>97</v>
-      </c>
-      <c r="C99">
-        <v>41</v>
-      </c>
-      <c r="D99">
-        <f t="shared" si="1"/>
-        <v>185</v>
       </c>
       <c r="E99">
         <v>21.10454545</v>
@@ -2759,19 +2759,19 @@
         <v>85.527272730000007</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>47</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100">
+        <v>18</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="D100" s="1">
         <v>98</v>
-      </c>
-      <c r="C100">
-        <v>18</v>
-      </c>
-      <c r="D100">
-        <f t="shared" si="1"/>
-        <v>163</v>
       </c>
       <c r="E100">
         <v>5.4738461540000003</v>
@@ -2783,19 +2783,19 @@
         <v>64.94923077</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>31</v>
       </c>
-      <c r="B101" s="1">
+      <c r="B101">
+        <v>11</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D101" s="1">
         <v>99</v>
-      </c>
-      <c r="C101">
-        <v>11</v>
-      </c>
-      <c r="D101">
-        <f t="shared" si="1"/>
-        <v>141</v>
       </c>
       <c r="E101">
         <v>7.8309523810000004</v>
@@ -2807,19 +2807,19 @@
         <v>63.654761899999997</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>33</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102">
+        <v>13</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D102" s="1">
         <v>100</v>
-      </c>
-      <c r="C102">
-        <v>13</v>
-      </c>
-      <c r="D102">
-        <f t="shared" si="1"/>
-        <v>146</v>
       </c>
       <c r="E102">
         <v>6.9804347829999998</v>
@@ -2831,19 +2831,19 @@
         <v>74.063043480000005</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>48</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103">
+        <v>7</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="D103" s="1">
         <v>101</v>
-      </c>
-      <c r="C103">
-        <v>7</v>
-      </c>
-      <c r="D103">
-        <f t="shared" si="1"/>
-        <v>156</v>
       </c>
       <c r="E103">
         <v>10.57454545</v>
@@ -2855,19 +2855,19 @@
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>33</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104">
+        <v>14</v>
+      </c>
+      <c r="C104">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D104" s="1">
         <v>102</v>
-      </c>
-      <c r="C104">
-        <v>14</v>
-      </c>
-      <c r="D104">
-        <f t="shared" si="1"/>
-        <v>149</v>
       </c>
       <c r="E104">
         <v>5.5</v>
@@ -2879,19 +2879,19 @@
         <v>78.961702130000006</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>20</v>
       </c>
-      <c r="B105" s="1">
+      <c r="B105">
+        <v>10</v>
+      </c>
+      <c r="C105">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D105" s="1">
         <v>103</v>
-      </c>
-      <c r="C105">
-        <v>10</v>
-      </c>
-      <c r="D105">
-        <f t="shared" si="1"/>
-        <v>133</v>
       </c>
       <c r="E105">
         <v>8.4499999999999993</v>

</xml_diff>

<commit_message>
atleast, atmost, exactly implemented
</commit_message>
<xml_diff>
--- a/org.xtext.example.Adeptness/resources/TrainingData_MiercolesSur_trainingdata1.xlsx
+++ b/org.xtext.example.Adeptness/resources/TrainingData_MiercolesSur_trainingdata1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\AdeptnessDSL\org.xtext.example.Adeptness\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E14937-52AB-4221-B529-10F5D60852F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36120EAC-36B3-4887-BE4C-21CBD87B1DFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27720" yWindow="1080" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>UP</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>timestamp</t>
+  </si>
+  <si>
+    <t>TEST_TIMING_COND_WHEN</t>
+  </si>
+  <si>
+    <t>TEST_TIMING_SIGNAL</t>
   </si>
 </sst>
 </file>
@@ -373,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -384,7 +390,7 @@
     <col min="4" max="4" width="10.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,8 +412,14 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>6</v>
       </c>
@@ -415,7 +427,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <f>SUM(A2:B2)</f>
+        <f t="shared" ref="C2:C33" si="0">SUM(A2:B2)</f>
         <v>6</v>
       </c>
       <c r="D2" s="1">
@@ -430,8 +442,14 @@
       <c r="G2">
         <v>57.483333330000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>4</v>
       </c>
@@ -439,7 +457,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f>SUM(A3:B3)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D3" s="1">
@@ -454,8 +472,14 @@
       <c r="G3">
         <v>43.483333330000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>8</v>
       </c>
@@ -463,7 +487,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <f>SUM(A4:B4)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="D4" s="1">
@@ -478,8 +502,14 @@
       <c r="G4">
         <v>46.044444439999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>7</v>
       </c>
@@ -487,7 +517,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <f>SUM(A5:B5)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D5" s="1">
@@ -502,8 +532,14 @@
       <c r="G5">
         <v>70.571428569999995</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>8</v>
       </c>
@@ -511,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <f>SUM(A6:B6)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D6" s="1">
@@ -526,8 +562,14 @@
       <c r="G6">
         <v>67.650000000000006</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>10</v>
       </c>
@@ -535,7 +577,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f>SUM(A7:B7)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D7" s="1">
@@ -550,8 +592,14 @@
       <c r="G7">
         <v>74.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
@@ -559,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <f>SUM(A8:B8)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D8" s="1">
@@ -574,8 +622,14 @@
       <c r="G8">
         <v>61.55</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9</v>
       </c>
@@ -583,7 +637,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <f>SUM(A9:B9)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D9" s="1">
@@ -598,8 +652,14 @@
       <c r="G9">
         <v>61.18</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -607,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <f>SUM(A10:B10)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D10" s="1">
@@ -622,8 +682,14 @@
       <c r="G10">
         <v>66.94</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>14</v>
       </c>
@@ -631,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f>SUM(A11:B11)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="D11" s="1">
@@ -646,8 +712,14 @@
       <c r="G11">
         <v>71.142857140000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>13</v>
       </c>
@@ -655,7 +727,7 @@
         <v>4</v>
       </c>
       <c r="C12">
-        <f>SUM(A12:B12)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="D12" s="1">
@@ -670,8 +742,14 @@
       <c r="G12">
         <v>77.92352941</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>18</v>
       </c>
@@ -679,7 +757,7 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <f>SUM(A13:B13)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="D13" s="1">
@@ -694,8 +772,14 @@
       <c r="G13">
         <v>63.185000000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>18</v>
       </c>
@@ -703,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <f>SUM(A14:B14)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="D14" s="1">
@@ -718,8 +802,14 @@
       <c r="G14">
         <v>96.984210529999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>23</v>
       </c>
@@ -727,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>SUM(A15:B15)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="D15" s="1">
@@ -742,8 +832,14 @@
       <c r="G15">
         <v>91.96086957</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>25</v>
       </c>
@@ -751,7 +847,7 @@
         <v>5</v>
       </c>
       <c r="C16">
-        <f>SUM(A16:B16)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="D16" s="1">
@@ -766,8 +862,14 @@
       <c r="G16">
         <v>75.05</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>29</v>
       </c>
@@ -775,7 +877,7 @@
         <v>2</v>
       </c>
       <c r="C17">
-        <f>SUM(A17:B17)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="D17" s="1">
@@ -790,8 +892,14 @@
       <c r="G17">
         <v>91.132258059999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>26</v>
       </c>
@@ -799,7 +907,7 @@
         <v>4</v>
       </c>
       <c r="C18">
-        <f>SUM(A18:B18)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="D18" s="1">
@@ -814,8 +922,14 @@
       <c r="G18">
         <v>73.16</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>25</v>
       </c>
@@ -823,7 +937,7 @@
         <v>2</v>
       </c>
       <c r="C19">
-        <f>SUM(A19:B19)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="D19" s="1">
@@ -838,8 +952,14 @@
       <c r="G19">
         <v>69.385185190000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>33</v>
       </c>
@@ -847,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <f>SUM(A20:B20)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="D20" s="1">
@@ -862,8 +982,14 @@
       <c r="G20">
         <v>91.573529410000006</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>38</v>
       </c>
@@ -871,7 +997,7 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <f>SUM(A21:B21)</f>
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="D21" s="1">
@@ -886,8 +1012,14 @@
       <c r="G21">
         <v>92.897560979999994</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>30</v>
       </c>
@@ -895,7 +1027,7 @@
         <v>5</v>
       </c>
       <c r="C22">
-        <f>SUM(A22:B22)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="D22" s="1">
@@ -910,8 +1042,14 @@
       <c r="G22">
         <v>77.58</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>25</v>
       </c>
@@ -919,7 +1057,7 @@
         <v>4</v>
       </c>
       <c r="C23">
-        <f>SUM(A23:B23)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="D23" s="1">
@@ -934,8 +1072,14 @@
       <c r="G23">
         <v>69.993103450000007</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>38</v>
       </c>
@@ -943,7 +1087,7 @@
         <v>5</v>
       </c>
       <c r="C24">
-        <f>SUM(A24:B24)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="D24" s="1">
@@ -958,8 +1102,14 @@
       <c r="G24">
         <v>92.844186050000005</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>40</v>
       </c>
@@ -967,7 +1117,7 @@
         <v>4</v>
       </c>
       <c r="C25">
-        <f>SUM(A25:B25)</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="D25" s="1">
@@ -982,8 +1132,14 @@
       <c r="G25">
         <v>82.109090910000006</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>40</v>
       </c>
@@ -991,7 +1147,7 @@
         <v>5</v>
       </c>
       <c r="C26">
-        <f>SUM(A26:B26)</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="D26" s="1">
@@ -1006,8 +1162,14 @@
       <c r="G26">
         <v>93.657777780000004</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>59</v>
       </c>
@@ -1015,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="C27">
-        <f>SUM(A27:B27)</f>
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="D27" s="1">
@@ -1030,8 +1192,14 @@
       <c r="G27">
         <v>113.9115942</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>44</v>
       </c>
@@ -1039,7 +1207,7 @@
         <v>3</v>
       </c>
       <c r="C28">
-        <f>SUM(A28:B28)</f>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="D28" s="1">
@@ -1054,8 +1222,14 @@
       <c r="G28">
         <v>113.46595739999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>47</v>
       </c>
@@ -1063,7 +1237,7 @@
         <v>4</v>
       </c>
       <c r="C29">
-        <f>SUM(A29:B29)</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="D29" s="1">
@@ -1078,8 +1252,14 @@
       <c r="G29">
         <v>89.627450980000006</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>44</v>
       </c>
@@ -1087,7 +1267,7 @@
         <v>11</v>
       </c>
       <c r="C30">
-        <f>SUM(A30:B30)</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="D30" s="1">
@@ -1102,8 +1282,14 @@
       <c r="G30">
         <v>88.598181819999994</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>59</v>
       </c>
@@ -1111,7 +1297,7 @@
         <v>10</v>
       </c>
       <c r="C31">
-        <f>SUM(A31:B31)</f>
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="D31" s="1">
@@ -1126,8 +1312,14 @@
       <c r="G31">
         <v>101.1304348</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>46</v>
       </c>
@@ -1135,7 +1327,7 @@
         <v>11</v>
       </c>
       <c r="C32">
-        <f>SUM(A32:B32)</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="D32" s="1">
@@ -1150,8 +1342,14 @@
       <c r="G32">
         <v>89.331578949999994</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>42</v>
       </c>
@@ -1159,7 +1357,7 @@
         <v>12</v>
       </c>
       <c r="C33">
-        <f>SUM(A33:B33)</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="D33" s="1">
@@ -1174,8 +1372,14 @@
       <c r="G33">
         <v>82.916666669999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>56</v>
       </c>
@@ -1183,7 +1387,7 @@
         <v>14</v>
       </c>
       <c r="C34">
-        <f>SUM(A34:B34)</f>
+        <f t="shared" ref="C34:C65" si="1">SUM(A34:B34)</f>
         <v>70</v>
       </c>
       <c r="D34" s="1">
@@ -1198,8 +1402,14 @@
       <c r="G34">
         <v>95.05285714</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>41</v>
       </c>
@@ -1207,7 +1417,7 @@
         <v>11</v>
       </c>
       <c r="C35">
-        <f>SUM(A35:B35)</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="D35" s="1">
@@ -1222,8 +1432,14 @@
       <c r="G35">
         <v>83.136538459999997</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>39</v>
       </c>
@@ -1231,7 +1447,7 @@
         <v>11</v>
       </c>
       <c r="C36">
-        <f>SUM(A36:B36)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="D36" s="1">
@@ -1246,8 +1462,14 @@
       <c r="G36">
         <v>89.278000000000006</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>53</v>
       </c>
@@ -1255,7 +1477,7 @@
         <v>20</v>
       </c>
       <c r="C37">
-        <f>SUM(A37:B37)</f>
+        <f t="shared" si="1"/>
         <v>73</v>
       </c>
       <c r="D37" s="1">
@@ -1270,8 +1492,14 @@
       <c r="G37">
         <v>84.006849320000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>39</v>
       </c>
@@ -1279,7 +1507,7 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <f>SUM(A38:B38)</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="D38" s="1">
@@ -1294,8 +1522,14 @@
       <c r="G38">
         <v>74.43090909</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1303,7 +1537,7 @@
         <v>15</v>
       </c>
       <c r="C39">
-        <f>SUM(A39:B39)</f>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="D39" s="1">
@@ -1318,8 +1552,14 @@
       <c r="G39">
         <v>65.969811320000005</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1327,7 +1567,7 @@
         <v>16</v>
       </c>
       <c r="C40">
-        <f>SUM(A40:B40)</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="D40" s="1">
@@ -1342,8 +1582,14 @@
       <c r="G40">
         <v>65.622222219999998</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>21</v>
       </c>
@@ -1351,7 +1597,7 @@
         <v>14</v>
       </c>
       <c r="C41">
-        <f>SUM(A41:B41)</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="D41" s="1">
@@ -1366,8 +1612,14 @@
       <c r="G41">
         <v>66.16857143</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>24</v>
       </c>
@@ -1375,7 +1627,7 @@
         <v>10</v>
       </c>
       <c r="C42">
-        <f>SUM(A42:B42)</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="D42" s="1">
@@ -1390,8 +1642,14 @@
       <c r="G42">
         <v>65.667647059999993</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>32</v>
       </c>
@@ -1399,7 +1657,7 @@
         <v>17</v>
       </c>
       <c r="C43">
-        <f>SUM(A43:B43)</f>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="D43" s="1">
@@ -1414,8 +1672,14 @@
       <c r="G43">
         <v>56.053061219999996</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>23</v>
       </c>
@@ -1423,7 +1687,7 @@
         <v>13</v>
       </c>
       <c r="C44">
-        <f>SUM(A44:B44)</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="D44" s="1">
@@ -1438,8 +1702,14 @@
       <c r="G44">
         <v>67.916666669999998</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>24</v>
       </c>
@@ -1447,7 +1717,7 @@
         <v>17</v>
       </c>
       <c r="C45">
-        <f>SUM(A45:B45)</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="D45" s="1">
@@ -1462,8 +1732,14 @@
       <c r="G45">
         <v>54.1</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>28</v>
       </c>
@@ -1471,7 +1747,7 @@
         <v>16</v>
       </c>
       <c r="C46">
-        <f>SUM(A46:B46)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="D46" s="1">
@@ -1486,8 +1762,14 @@
       <c r="G46">
         <v>64.963636359999995</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>10</v>
       </c>
@@ -1495,7 +1777,7 @@
         <v>19</v>
       </c>
       <c r="C47">
-        <f>SUM(A47:B47)</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="D47" s="1">
@@ -1510,8 +1792,14 @@
       <c r="G47">
         <v>46.25517241</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>27</v>
       </c>
@@ -1519,7 +1807,7 @@
         <v>24</v>
       </c>
       <c r="C48">
-        <f>SUM(A48:B48)</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="D48" s="1">
@@ -1534,8 +1822,14 @@
       <c r="G48">
         <v>54.523529410000002</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>24</v>
       </c>
@@ -1543,7 +1837,7 @@
         <v>36</v>
       </c>
       <c r="C49">
-        <f>SUM(A49:B49)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="D49" s="1">
@@ -1558,8 +1852,14 @@
       <c r="G49">
         <v>67.709999999999994</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>28</v>
       </c>
@@ -1567,7 +1867,7 @@
         <v>14</v>
       </c>
       <c r="C50">
-        <f>SUM(A50:B50)</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="D50" s="1">
@@ -1582,8 +1882,14 @@
       <c r="G50">
         <v>77.209523809999993</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>27</v>
       </c>
@@ -1591,7 +1897,7 @@
         <v>24</v>
       </c>
       <c r="C51">
-        <f>SUM(A51:B51)</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="D51" s="1">
@@ -1606,8 +1912,14 @@
       <c r="G51">
         <v>64.372549019999994</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>27</v>
       </c>
@@ -1615,7 +1927,7 @@
         <v>28</v>
       </c>
       <c r="C52">
-        <f>SUM(A52:B52)</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="D52" s="1">
@@ -1630,8 +1942,14 @@
       <c r="G52">
         <v>82.532727269999995</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>18</v>
       </c>
@@ -1639,7 +1957,7 @@
         <v>26</v>
       </c>
       <c r="C53">
-        <f>SUM(A53:B53)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="D53" s="1">
@@ -1654,8 +1972,14 @@
       <c r="G53">
         <v>58.465909089999997</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>14</v>
       </c>
@@ -1663,7 +1987,7 @@
         <v>13</v>
       </c>
       <c r="C54">
-        <f>SUM(A54:B54)</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="D54" s="1">
@@ -1678,8 +2002,14 @@
       <c r="G54">
         <v>55.611111110000003</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>23</v>
       </c>
@@ -1687,7 +2017,7 @@
         <v>18</v>
       </c>
       <c r="C55">
-        <f>SUM(A55:B55)</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="D55" s="1">
@@ -1702,8 +2032,14 @@
       <c r="G55">
         <v>65.041463410000006</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>25</v>
       </c>
@@ -1711,7 +2047,7 @@
         <v>17</v>
       </c>
       <c r="C56">
-        <f>SUM(A56:B56)</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="D56" s="1">
@@ -1726,8 +2062,14 @@
       <c r="G56">
         <v>56.580952379999999</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>21</v>
       </c>
@@ -1735,7 +2077,7 @@
         <v>17</v>
       </c>
       <c r="C57">
-        <f>SUM(A57:B57)</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="D57" s="1">
@@ -1750,8 +2092,14 @@
       <c r="G57">
         <v>52.05</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>31</v>
       </c>
@@ -1759,7 +2107,7 @@
         <v>12</v>
       </c>
       <c r="C58">
-        <f>SUM(A58:B58)</f>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="D58" s="1">
@@ -1774,8 +2122,14 @@
       <c r="G58">
         <v>60.511627910000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>11</v>
       </c>
@@ -1783,7 +2137,7 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <f>SUM(A59:B59)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="D59" s="1">
@@ -1798,8 +2152,14 @@
       <c r="G59">
         <v>50.7</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>23</v>
       </c>
@@ -1807,7 +2167,7 @@
         <v>20</v>
       </c>
       <c r="C60">
-        <f>SUM(A60:B60)</f>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="D60" s="1">
@@ -1822,8 +2182,14 @@
       <c r="G60">
         <v>55.68372093</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>26</v>
       </c>
@@ -1831,7 +2197,7 @@
         <v>20</v>
       </c>
       <c r="C61">
-        <f>SUM(A61:B61)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="D61" s="1">
@@ -1846,8 +2212,14 @@
       <c r="G61">
         <v>61.867391300000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>30</v>
       </c>
@@ -1855,7 +2227,7 @@
         <v>35</v>
       </c>
       <c r="C62">
-        <f>SUM(A62:B62)</f>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="D62" s="1">
@@ -1870,8 +2242,14 @@
       <c r="G62">
         <v>67.066153850000006</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>32</v>
       </c>
@@ -1879,7 +2257,7 @@
         <v>20</v>
       </c>
       <c r="C63">
-        <f>SUM(A63:B63)</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="D63" s="1">
@@ -1894,8 +2272,14 @@
       <c r="G63">
         <v>70.105769230000007</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>28</v>
       </c>
@@ -1903,7 +2287,7 @@
         <v>7</v>
       </c>
       <c r="C64">
-        <f>SUM(A64:B64)</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="D64" s="1">
@@ -1918,8 +2302,14 @@
       <c r="G64">
         <v>51.737142859999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>26</v>
       </c>
@@ -1927,7 +2317,7 @@
         <v>19</v>
       </c>
       <c r="C65">
-        <f>SUM(A65:B65)</f>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="D65" s="1">
@@ -1942,8 +2332,14 @@
       <c r="G65">
         <v>51.82222222</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>22</v>
       </c>
@@ -1951,7 +2347,7 @@
         <v>23</v>
       </c>
       <c r="C66">
-        <f>SUM(A66:B66)</f>
+        <f t="shared" ref="C66" si="2">SUM(A66:B66)</f>
         <v>45</v>
       </c>
       <c r="D66" s="1">
@@ -1966,8 +2362,14 @@
       <c r="G66">
         <v>58.455555560000001</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>8</v>
       </c>
@@ -1975,7 +2377,7 @@
         <v>13</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C105" si="0">SUM(A67:B67)</f>
+        <f t="shared" ref="C67:C105" si="3">SUM(A67:B67)</f>
         <v>21</v>
       </c>
       <c r="D67" s="1">
@@ -1990,8 +2392,14 @@
       <c r="G67">
         <v>48.985714289999997</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>13</v>
       </c>
@@ -1999,7 +2407,7 @@
         <v>13</v>
       </c>
       <c r="C68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="D68" s="1">
@@ -2014,8 +2422,14 @@
       <c r="G68">
         <v>52.157692310000002</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>23</v>
       </c>
@@ -2023,7 +2437,7 @@
         <v>8</v>
       </c>
       <c r="C69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="D69" s="1">
@@ -2038,8 +2452,14 @@
       <c r="G69">
         <v>55.603225809999998</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>14</v>
       </c>
@@ -2047,7 +2467,7 @@
         <v>25</v>
       </c>
       <c r="C70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="D70" s="1">
@@ -2062,8 +2482,14 @@
       <c r="G70">
         <v>64.851282049999995</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>8</v>
       </c>
@@ -2071,7 +2497,7 @@
         <v>14</v>
       </c>
       <c r="C71">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="D71" s="1">
@@ -2086,8 +2512,14 @@
       <c r="G71">
         <v>64.363636360000001</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>12</v>
       </c>
@@ -2095,7 +2527,7 @@
         <v>6</v>
       </c>
       <c r="C72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="D72" s="1">
@@ -2110,8 +2542,14 @@
       <c r="G72">
         <v>46.022222220000003</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>14</v>
       </c>
@@ -2119,7 +2557,7 @@
         <v>20</v>
       </c>
       <c r="C73">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="D73" s="1">
@@ -2134,8 +2572,14 @@
       <c r="G73">
         <v>59.232352939999998</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>20</v>
       </c>
@@ -2143,7 +2587,7 @@
         <v>37</v>
       </c>
       <c r="C74">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="D74" s="1">
@@ -2158,8 +2602,14 @@
       <c r="G74">
         <v>68.064912280000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>16</v>
       </c>
@@ -2167,7 +2617,7 @@
         <v>45</v>
       </c>
       <c r="C75">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>61</v>
       </c>
       <c r="D75" s="1">
@@ -2182,8 +2632,14 @@
       <c r="G75">
         <v>74.572131150000004</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>15</v>
       </c>
@@ -2191,7 +2647,7 @@
         <v>30</v>
       </c>
       <c r="C76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="D76" s="1">
@@ -2206,8 +2662,14 @@
       <c r="G76">
         <v>60.5</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>21</v>
       </c>
@@ -2215,7 +2677,7 @@
         <v>41</v>
       </c>
       <c r="C77">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
       <c r="D77" s="1">
@@ -2230,8 +2692,14 @@
       <c r="G77">
         <v>67.301612899999995</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>8</v>
       </c>
@@ -2239,7 +2707,7 @@
         <v>33</v>
       </c>
       <c r="C78">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="D78" s="1">
@@ -2254,8 +2722,14 @@
       <c r="G78">
         <v>63.897560980000002</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>10</v>
       </c>
@@ -2263,7 +2737,7 @@
         <v>43</v>
       </c>
       <c r="C79">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>53</v>
       </c>
       <c r="D79" s="1">
@@ -2278,8 +2752,14 @@
       <c r="G79">
         <v>60.354716979999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>16</v>
       </c>
@@ -2287,7 +2767,7 @@
         <v>35</v>
       </c>
       <c r="C80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
       <c r="D80" s="1">
@@ -2302,8 +2782,14 @@
       <c r="G80">
         <v>55.913725489999997</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>19</v>
       </c>
@@ -2311,7 +2797,7 @@
         <v>28</v>
       </c>
       <c r="C81">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="D81" s="1">
@@ -2326,8 +2812,14 @@
       <c r="G81">
         <v>58.861702129999998</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>19</v>
       </c>
@@ -2335,7 +2827,7 @@
         <v>33</v>
       </c>
       <c r="C82">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="D82" s="1">
@@ -2350,8 +2842,14 @@
       <c r="G82">
         <v>61.146153849999997</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>12</v>
       </c>
@@ -2359,7 +2857,7 @@
         <v>51</v>
       </c>
       <c r="C83">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
       <c r="D83" s="1">
@@ -2374,8 +2872,14 @@
       <c r="G83">
         <v>60.882539680000001</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>18</v>
       </c>
@@ -2383,7 +2887,7 @@
         <v>18</v>
       </c>
       <c r="C84">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="D84" s="1">
@@ -2398,8 +2902,14 @@
       <c r="G84">
         <v>55.013888889999997</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>19</v>
       </c>
@@ -2407,7 +2917,7 @@
         <v>26</v>
       </c>
       <c r="C85">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="D85" s="1">
@@ -2422,8 +2932,14 @@
       <c r="G85">
         <v>60.77333333</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>35</v>
       </c>
@@ -2431,7 +2947,7 @@
         <v>58</v>
       </c>
       <c r="C86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>93</v>
       </c>
       <c r="D86" s="1">
@@ -2446,8 +2962,14 @@
       <c r="G86">
         <v>64.358064519999999</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>32</v>
       </c>
@@ -2455,7 +2977,7 @@
         <v>49</v>
       </c>
       <c r="C87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="D87" s="1">
@@ -2470,8 +2992,14 @@
       <c r="G87">
         <v>67.758024689999999</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H87">
+        <v>0</v>
+      </c>
+      <c r="I87">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>31</v>
       </c>
@@ -2479,7 +3007,7 @@
         <v>43</v>
       </c>
       <c r="C88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>74</v>
       </c>
       <c r="D88" s="1">
@@ -2494,8 +3022,14 @@
       <c r="G88">
         <v>86.524324320000005</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>60</v>
       </c>
@@ -2503,7 +3037,7 @@
         <v>44</v>
       </c>
       <c r="C89">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
       <c r="D89" s="1">
@@ -2518,8 +3052,14 @@
       <c r="G89">
         <v>94.474038460000003</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>37</v>
       </c>
@@ -2527,7 +3067,7 @@
         <v>23</v>
       </c>
       <c r="C90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="D90" s="1">
@@ -2542,8 +3082,14 @@
       <c r="G90">
         <v>62.806666669999998</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>42</v>
       </c>
@@ -2551,7 +3097,7 @@
         <v>21</v>
       </c>
       <c r="C91">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
       <c r="D91" s="1">
@@ -2566,8 +3112,14 @@
       <c r="G91">
         <v>70.238095240000007</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>18</v>
       </c>
@@ -2575,7 +3127,7 @@
         <v>24</v>
       </c>
       <c r="C92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="D92" s="1">
@@ -2590,8 +3142,14 @@
       <c r="G92">
         <v>61.128571430000001</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>15</v>
       </c>
@@ -2599,7 +3157,7 @@
         <v>20</v>
       </c>
       <c r="C93">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="D93" s="1">
@@ -2614,8 +3172,14 @@
       <c r="G93">
         <v>51.01714286</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>21</v>
       </c>
@@ -2623,7 +3187,7 @@
         <v>11</v>
       </c>
       <c r="C94">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="D94" s="1">
@@ -2638,8 +3202,14 @@
       <c r="G94">
         <v>58.174999999999997</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>23</v>
       </c>
@@ -2647,7 +3217,7 @@
         <v>15</v>
       </c>
       <c r="C95">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="D95" s="1">
@@ -2662,8 +3232,14 @@
       <c r="G95">
         <v>71.281578949999997</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>21</v>
       </c>
@@ -2671,7 +3247,7 @@
         <v>7</v>
       </c>
       <c r="C96">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="D96" s="1">
@@ -2686,8 +3262,14 @@
       <c r="G96">
         <v>61.553571429999998</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>32</v>
       </c>
@@ -2695,7 +3277,7 @@
         <v>19</v>
       </c>
       <c r="C97">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
       <c r="D97" s="1">
@@ -2710,8 +3292,14 @@
       <c r="G97">
         <v>72.094117650000001</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>74</v>
       </c>
@@ -2719,7 +3307,7 @@
         <v>39</v>
       </c>
       <c r="C98">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>113</v>
       </c>
       <c r="D98" s="1">
@@ -2734,8 +3322,14 @@
       <c r="G98">
         <v>91.475221239999996</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>47</v>
       </c>
@@ -2743,7 +3337,7 @@
         <v>41</v>
       </c>
       <c r="C99">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>88</v>
       </c>
       <c r="D99" s="1">
@@ -2758,8 +3352,14 @@
       <c r="G99">
         <v>85.527272730000007</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>47</v>
       </c>
@@ -2767,7 +3367,7 @@
         <v>18</v>
       </c>
       <c r="C100">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="D100" s="1">
@@ -2782,8 +3382,14 @@
       <c r="G100">
         <v>64.94923077</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>31</v>
       </c>
@@ -2791,7 +3397,7 @@
         <v>11</v>
       </c>
       <c r="C101">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="D101" s="1">
@@ -2806,8 +3412,14 @@
       <c r="G101">
         <v>63.654761899999997</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>33</v>
       </c>
@@ -2815,7 +3427,7 @@
         <v>13</v>
       </c>
       <c r="C102">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="D102" s="1">
@@ -2830,8 +3442,14 @@
       <c r="G102">
         <v>74.063043480000005</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>48</v>
       </c>
@@ -2839,7 +3457,7 @@
         <v>7</v>
       </c>
       <c r="C103">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="D103" s="1">
@@ -2854,8 +3472,14 @@
       <c r="G103">
         <v>80</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H103">
+        <v>0</v>
+      </c>
+      <c r="I103">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>33</v>
       </c>
@@ -2863,7 +3487,7 @@
         <v>14</v>
       </c>
       <c r="C104">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="D104" s="1">
@@ -2878,8 +3502,14 @@
       <c r="G104">
         <v>78.961702130000006</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H104">
+        <v>0</v>
+      </c>
+      <c r="I104">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>20</v>
       </c>
@@ -2887,7 +3517,7 @@
         <v>10</v>
       </c>
       <c r="C105">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="D105" s="1">
@@ -2901,6 +3531,12 @@
       </c>
       <c r="G105">
         <v>54.426666670000003</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix boolean variables normalization
</commit_message>
<xml_diff>
--- a/org.xtext.example.Adeptness/resources/TrainingData_MiercolesSur_trainingdata1.xlsx
+++ b/org.xtext.example.Adeptness/resources/TrainingData_MiercolesSur_trainingdata1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\AdeptnessDSL\org.xtext.example.Adeptness\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\AdeptnessDSLclean\org.xtext.example.Adeptness\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36120EAC-36B3-4887-BE4C-21CBD87B1DFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46118B75-C526-4019-96BE-AE0D52321DF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>UP</t>
   </si>
@@ -62,13 +62,24 @@
   <si>
     <t>TEST_TIMING_SIGNAL</t>
   </si>
+  <si>
+    <t>TEST_BOOLEAN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -96,9 +107,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,18 +392,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="J105" sqref="J105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="10.90625" style="1"/>
+    <col min="11" max="11" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,8 +432,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>6</v>
       </c>
@@ -448,8 +465,11 @@
       <c r="I2">
         <v>110</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>4</v>
       </c>
@@ -478,8 +498,11 @@
       <c r="I3">
         <v>109</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>8</v>
       </c>
@@ -508,8 +531,11 @@
       <c r="I4">
         <v>108</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>7</v>
       </c>
@@ -538,8 +564,11 @@
       <c r="I5">
         <v>107</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>8</v>
       </c>
@@ -568,8 +597,11 @@
       <c r="I6">
         <v>106</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>10</v>
       </c>
@@ -598,8 +630,12 @@
       <c r="I7">
         <v>105</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
@@ -628,8 +664,11 @@
       <c r="I8">
         <v>104</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9</v>
       </c>
@@ -658,8 +697,11 @@
       <c r="I9">
         <v>103</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -688,8 +730,11 @@
       <c r="I10">
         <v>102</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>14</v>
       </c>
@@ -718,8 +763,11 @@
       <c r="I11">
         <v>101</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>13</v>
       </c>
@@ -748,8 +796,11 @@
       <c r="I12">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>18</v>
       </c>
@@ -778,8 +829,11 @@
       <c r="I13">
         <v>99</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>18</v>
       </c>
@@ -808,8 +862,11 @@
       <c r="I14">
         <v>98</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>23</v>
       </c>
@@ -838,8 +895,11 @@
       <c r="I15">
         <v>97</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>25</v>
       </c>
@@ -868,8 +928,11 @@
       <c r="I16">
         <v>96</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>29</v>
       </c>
@@ -898,8 +961,11 @@
       <c r="I17">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>26</v>
       </c>
@@ -928,8 +994,11 @@
       <c r="I18">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>25</v>
       </c>
@@ -958,8 +1027,11 @@
       <c r="I19">
         <v>93</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>33</v>
       </c>
@@ -988,8 +1060,11 @@
       <c r="I20">
         <v>92</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>38</v>
       </c>
@@ -1018,8 +1093,11 @@
       <c r="I21">
         <v>91</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>30</v>
       </c>
@@ -1048,8 +1126,11 @@
       <c r="I22">
         <v>90</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>25</v>
       </c>
@@ -1078,8 +1159,11 @@
       <c r="I23">
         <v>89</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>38</v>
       </c>
@@ -1108,8 +1192,11 @@
       <c r="I24">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>40</v>
       </c>
@@ -1138,8 +1225,11 @@
       <c r="I25">
         <v>87</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>40</v>
       </c>
@@ -1168,8 +1258,11 @@
       <c r="I26">
         <v>86</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>59</v>
       </c>
@@ -1198,8 +1291,11 @@
       <c r="I27">
         <v>85</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>44</v>
       </c>
@@ -1228,8 +1324,11 @@
       <c r="I28">
         <v>84</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>47</v>
       </c>
@@ -1258,8 +1357,11 @@
       <c r="I29">
         <v>83</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>44</v>
       </c>
@@ -1288,8 +1390,11 @@
       <c r="I30">
         <v>82</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>59</v>
       </c>
@@ -1318,8 +1423,11 @@
       <c r="I31">
         <v>81</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>46</v>
       </c>
@@ -1348,8 +1456,11 @@
       <c r="I32">
         <v>80</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>42</v>
       </c>
@@ -1378,8 +1489,11 @@
       <c r="I33">
         <v>79</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>56</v>
       </c>
@@ -1408,8 +1522,11 @@
       <c r="I34">
         <v>78</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>41</v>
       </c>
@@ -1438,8 +1555,11 @@
       <c r="I35">
         <v>77</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J35" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>39</v>
       </c>
@@ -1468,8 +1588,11 @@
       <c r="I36">
         <v>76</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J36" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>53</v>
       </c>
@@ -1498,8 +1621,11 @@
       <c r="I37">
         <v>75</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>39</v>
       </c>
@@ -1528,8 +1654,11 @@
       <c r="I38">
         <v>74</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J38" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1558,8 +1687,11 @@
       <c r="I39">
         <v>73</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1588,8 +1720,11 @@
       <c r="I40">
         <v>72</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>21</v>
       </c>
@@ -1618,8 +1753,11 @@
       <c r="I41">
         <v>71</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J41" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>24</v>
       </c>
@@ -1648,8 +1786,11 @@
       <c r="I42">
         <v>70</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>32</v>
       </c>
@@ -1678,8 +1819,11 @@
       <c r="I43">
         <v>69</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J43" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>23</v>
       </c>
@@ -1708,8 +1852,11 @@
       <c r="I44">
         <v>68</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>24</v>
       </c>
@@ -1738,8 +1885,11 @@
       <c r="I45">
         <v>67</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J45" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>28</v>
       </c>
@@ -1768,8 +1918,11 @@
       <c r="I46">
         <v>66</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>10</v>
       </c>
@@ -1798,8 +1951,11 @@
       <c r="I47">
         <v>65</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J47" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>27</v>
       </c>
@@ -1828,8 +1984,11 @@
       <c r="I48">
         <v>64</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>24</v>
       </c>
@@ -1858,8 +2017,11 @@
       <c r="I49">
         <v>63</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J49" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>28</v>
       </c>
@@ -1888,8 +2050,11 @@
       <c r="I50">
         <v>62</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J50" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>27</v>
       </c>
@@ -1918,8 +2083,11 @@
       <c r="I51">
         <v>61</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J51" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>27</v>
       </c>
@@ -1948,8 +2116,11 @@
       <c r="I52">
         <v>60</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>18</v>
       </c>
@@ -1978,8 +2149,11 @@
       <c r="I53">
         <v>59</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J53" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>14</v>
       </c>
@@ -2008,8 +2182,11 @@
       <c r="I54">
         <v>58</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>23</v>
       </c>
@@ -2038,8 +2215,11 @@
       <c r="I55">
         <v>57</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J55" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>25</v>
       </c>
@@ -2068,8 +2248,11 @@
       <c r="I56">
         <v>56</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>21</v>
       </c>
@@ -2098,8 +2281,11 @@
       <c r="I57">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J57" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>31</v>
       </c>
@@ -2128,8 +2314,11 @@
       <c r="I58">
         <v>54</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J58" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>11</v>
       </c>
@@ -2158,8 +2347,11 @@
       <c r="I59">
         <v>53</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J59" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>23</v>
       </c>
@@ -2188,8 +2380,11 @@
       <c r="I60">
         <v>52</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J60" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>26</v>
       </c>
@@ -2218,8 +2413,11 @@
       <c r="I61">
         <v>51</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J61" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>30</v>
       </c>
@@ -2248,8 +2446,11 @@
       <c r="I62">
         <v>50</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J62" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>32</v>
       </c>
@@ -2278,8 +2479,11 @@
       <c r="I63">
         <v>49</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J63" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>28</v>
       </c>
@@ -2308,8 +2512,11 @@
       <c r="I64">
         <v>48</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J64" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>26</v>
       </c>
@@ -2338,8 +2545,11 @@
       <c r="I65">
         <v>47</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J65" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>22</v>
       </c>
@@ -2368,8 +2578,11 @@
       <c r="I66">
         <v>46</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J66" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>8</v>
       </c>
@@ -2398,8 +2611,11 @@
       <c r="I67">
         <v>45</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J67" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>13</v>
       </c>
@@ -2428,8 +2644,11 @@
       <c r="I68">
         <v>44</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>23</v>
       </c>
@@ -2458,8 +2677,11 @@
       <c r="I69">
         <v>43</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J69" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>14</v>
       </c>
@@ -2488,8 +2710,11 @@
       <c r="I70">
         <v>42</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J70" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>8</v>
       </c>
@@ -2518,8 +2743,11 @@
       <c r="I71">
         <v>41</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J71" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>12</v>
       </c>
@@ -2548,8 +2776,11 @@
       <c r="I72">
         <v>40</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J72" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>14</v>
       </c>
@@ -2578,8 +2809,11 @@
       <c r="I73">
         <v>39</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J73" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>20</v>
       </c>
@@ -2608,8 +2842,11 @@
       <c r="I74">
         <v>38</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J74" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>16</v>
       </c>
@@ -2638,8 +2875,11 @@
       <c r="I75">
         <v>37</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J75" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>15</v>
       </c>
@@ -2668,8 +2908,11 @@
       <c r="I76">
         <v>36</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J76" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>21</v>
       </c>
@@ -2698,8 +2941,11 @@
       <c r="I77">
         <v>35</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J77" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>8</v>
       </c>
@@ -2728,8 +2974,11 @@
       <c r="I78">
         <v>34</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J78" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>10</v>
       </c>
@@ -2758,8 +3007,11 @@
       <c r="I79">
         <v>33</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J79" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>16</v>
       </c>
@@ -2788,8 +3040,11 @@
       <c r="I80">
         <v>32</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J80" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>19</v>
       </c>
@@ -2818,8 +3073,11 @@
       <c r="I81">
         <v>31</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J81" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>19</v>
       </c>
@@ -2848,8 +3106,11 @@
       <c r="I82">
         <v>30</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J82" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>12</v>
       </c>
@@ -2878,8 +3139,11 @@
       <c r="I83">
         <v>29</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J83" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>18</v>
       </c>
@@ -2908,8 +3172,11 @@
       <c r="I84">
         <v>28</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J84" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>19</v>
       </c>
@@ -2938,8 +3205,11 @@
       <c r="I85">
         <v>27</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J85" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>35</v>
       </c>
@@ -2968,8 +3238,11 @@
       <c r="I86">
         <v>26</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J86" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>32</v>
       </c>
@@ -2998,8 +3271,11 @@
       <c r="I87">
         <v>25</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J87" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>31</v>
       </c>
@@ -3028,8 +3304,11 @@
       <c r="I88">
         <v>24</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J88" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>60</v>
       </c>
@@ -3058,8 +3337,11 @@
       <c r="I89">
         <v>23</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J89" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>37</v>
       </c>
@@ -3088,8 +3370,11 @@
       <c r="I90">
         <v>22</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J90" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>42</v>
       </c>
@@ -3118,8 +3403,11 @@
       <c r="I91">
         <v>21</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J91" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>18</v>
       </c>
@@ -3148,8 +3436,11 @@
       <c r="I92">
         <v>20</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J92" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>15</v>
       </c>
@@ -3178,8 +3469,11 @@
       <c r="I93">
         <v>19</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J93" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>21</v>
       </c>
@@ -3208,8 +3502,11 @@
       <c r="I94">
         <v>18</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J94" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>23</v>
       </c>
@@ -3238,8 +3535,11 @@
       <c r="I95">
         <v>17</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J95" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>21</v>
       </c>
@@ -3268,8 +3568,11 @@
       <c r="I96">
         <v>16</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J96" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>32</v>
       </c>
@@ -3298,8 +3601,11 @@
       <c r="I97">
         <v>15</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J97" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>74</v>
       </c>
@@ -3328,8 +3634,11 @@
       <c r="I98">
         <v>14</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J98" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>47</v>
       </c>
@@ -3358,8 +3667,11 @@
       <c r="I99">
         <v>13</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J99" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>47</v>
       </c>
@@ -3388,8 +3700,11 @@
       <c r="I100">
         <v>12</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J100" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>31</v>
       </c>
@@ -3418,8 +3733,11 @@
       <c r="I101">
         <v>11</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J101" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>33</v>
       </c>
@@ -3448,8 +3766,11 @@
       <c r="I102">
         <v>10</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J102" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>48</v>
       </c>
@@ -3478,8 +3799,11 @@
       <c r="I103">
         <v>9</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J103" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>33</v>
       </c>
@@ -3508,8 +3832,11 @@
       <c r="I104">
         <v>8</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J104" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>20</v>
       </c>
@@ -3537,6 +3864,9 @@
       </c>
       <c r="I105">
         <v>7</v>
+      </c>
+      <c r="J105" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>